<commit_message>
Switched off scrambling articles, more results in xlsx
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad1/wyniki.xlsx
+++ b/Sprawozdanie_zad1/wyniki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C505A88F-7CF0-4A87-890E-875E9AD5C6E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65C828D-DC47-4C93-85A3-936B6318FD46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
   <si>
     <t>usa</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>85 / 15</t>
+  </si>
+  <si>
+    <t>nowe wynikimbez losowania , slowa kluczowe bez liczb i zn&lt;3</t>
+  </si>
+  <si>
+    <t>77 / 23</t>
+  </si>
+  <si>
+    <t>80 / 20</t>
   </si>
 </sst>
 </file>
@@ -217,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -236,6 +245,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -516,19 +528,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA61"/>
+  <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="AB36" sqref="AB36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5">
         <v>322</v>
       </c>
@@ -536,7 +549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>10685</v>
       </c>
@@ -611,7 +624,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>251</v>
       </c>
@@ -702,7 +715,7 @@
         <v>13440</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>905</v>
       </c>
@@ -710,7 +723,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>812</v>
       </c>
@@ -718,20 +731,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>466</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E7" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="R7" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E8" s="14" t="s">
         <v>7</v>
       </c>
@@ -765,8 +784,41 @@
       <c r="O8">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="R8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="S8">
+        <v>2</v>
+      </c>
+      <c r="T8">
+        <v>3</v>
+      </c>
+      <c r="U8">
+        <v>4</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+      <c r="W8">
+        <v>7</v>
+      </c>
+      <c r="X8">
+        <v>10</v>
+      </c>
+      <c r="Y8">
+        <v>13</v>
+      </c>
+      <c r="Z8">
+        <v>15</v>
+      </c>
+      <c r="AA8">
+        <v>20</v>
+      </c>
+      <c r="AB8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E9" s="14" t="s">
         <v>9</v>
       </c>
@@ -800,8 +852,41 @@
       <c r="O9" s="15">
         <v>0.79472770845384599</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="R9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="S9" s="15">
+        <v>0.65473927774564</v>
+      </c>
+      <c r="T9" s="15">
+        <v>0.73208825716882897</v>
+      </c>
+      <c r="U9" s="15">
+        <v>0.74836790347905102</v>
+      </c>
+      <c r="V9" s="15">
+        <v>0.77167176266424198</v>
+      </c>
+      <c r="W9" s="15">
+        <v>0.78456325923477399</v>
+      </c>
+      <c r="X9" s="15">
+        <v>0.79001735393769101</v>
+      </c>
+      <c r="Y9" s="15">
+        <v>0.79266176349062001</v>
+      </c>
+      <c r="Z9" s="15">
+        <v>0.79307495248326498</v>
+      </c>
+      <c r="AA9" s="15">
+        <v>0.79340550367738205</v>
+      </c>
+      <c r="AB9" s="15">
+        <v>0.79340550367738205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E10" s="14" t="s">
         <v>10</v>
       </c>
@@ -835,8 +920,19 @@
       <c r="O10" s="15">
         <v>0.79381869267002703</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -873,23 +969,39 @@
       <c r="O11" s="15">
         <v>0.79522353524502098</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P11" s="15"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P12" s="15"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P13" s="15"/>
+      <c r="R13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -926,8 +1038,42 @@
       <c r="O14">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P14" s="15"/>
+      <c r="R14" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="S14" s="19">
+        <v>2</v>
+      </c>
+      <c r="T14" s="19">
+        <v>3</v>
+      </c>
+      <c r="U14" s="19">
+        <v>4</v>
+      </c>
+      <c r="V14" s="19">
+        <v>5</v>
+      </c>
+      <c r="W14" s="19">
+        <v>7</v>
+      </c>
+      <c r="X14" s="19">
+        <v>10</v>
+      </c>
+      <c r="Y14" s="19">
+        <v>13</v>
+      </c>
+      <c r="Z14" s="19">
+        <v>15</v>
+      </c>
+      <c r="AA14" s="19">
+        <v>20</v>
+      </c>
+      <c r="AB14" s="19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -956,8 +1102,42 @@
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P15" s="15"/>
+      <c r="R15" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="S15" s="20">
+        <v>0.66192548561723796</v>
+      </c>
+      <c r="T15" s="20">
+        <v>0.72614372147330397</v>
+      </c>
+      <c r="U15" s="20">
+        <v>0.73813820188939605</v>
+      </c>
+      <c r="V15" s="20">
+        <v>0.75873049570109297</v>
+      </c>
+      <c r="W15" s="20">
+        <v>0.77560768495913401</v>
+      </c>
+      <c r="X15" s="20">
+        <v>0.779535081201571</v>
+      </c>
+      <c r="Y15" s="20">
+        <v>0.78707143615327402</v>
+      </c>
+      <c r="Z15" s="20">
+        <v>0.78983122810741901</v>
+      </c>
+      <c r="AA15" s="20">
+        <v>0.79068039486254105</v>
+      </c>
+      <c r="AB15" s="20">
+        <v>0.79407706188302696</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="17"/>
@@ -986,8 +1166,9 @@
       <c r="M16" s="15"/>
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P16" s="15"/>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B17" s="16" t="s">
         <v>12</v>
       </c>
@@ -1018,16 +1199,18 @@
       <c r="M17" s="15"/>
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P17" s="15"/>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B18" s="15">
         <v>0.77279375914188198</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="15"/>
       <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P18" s="15"/>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>13</v>
       </c>
@@ -1036,8 +1219,22 @@
       <c r="E19" s="14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P19" s="15"/>
+      <c r="R19" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="19"/>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="19"/>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B20" s="15">
         <v>0.79180887372013598</v>
       </c>
@@ -1076,8 +1273,42 @@
       <c r="O20">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P20" s="15"/>
+      <c r="R20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="S20" s="19">
+        <v>2</v>
+      </c>
+      <c r="T20" s="19">
+        <v>3</v>
+      </c>
+      <c r="U20" s="19">
+        <v>4</v>
+      </c>
+      <c r="V20" s="19">
+        <v>5</v>
+      </c>
+      <c r="W20" s="19">
+        <v>7</v>
+      </c>
+      <c r="X20" s="19">
+        <v>10</v>
+      </c>
+      <c r="Y20" s="19">
+        <v>13</v>
+      </c>
+      <c r="Z20" s="19">
+        <v>15</v>
+      </c>
+      <c r="AA20" s="19">
+        <v>20</v>
+      </c>
+      <c r="AB20" s="19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
         <v>14</v>
       </c>
@@ -1108,8 +1339,42 @@
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P21" s="15"/>
+      <c r="R21" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="S21" s="20">
+        <v>0.67141373683429695</v>
+      </c>
+      <c r="T21" s="20">
+        <v>0.72971369233051397</v>
+      </c>
+      <c r="U21" s="20">
+        <v>0.742471443406022</v>
+      </c>
+      <c r="V21" s="20">
+        <v>0.75789942145082301</v>
+      </c>
+      <c r="W21" s="20">
+        <v>0.77822281560599305</v>
+      </c>
+      <c r="X21" s="20">
+        <v>0.78742026405577803</v>
+      </c>
+      <c r="Y21" s="20">
+        <v>0.79261237205162405</v>
+      </c>
+      <c r="Z21" s="20">
+        <v>0.793502447708055</v>
+      </c>
+      <c r="AA21" s="20">
+        <v>0.79735944221925503</v>
+      </c>
+      <c r="AB21" s="20">
+        <v>0.79810117193294705</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B22" s="15">
         <v>0.79229644076060401</v>
       </c>
@@ -1140,8 +1405,9 @@
       <c r="M22" s="15"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P22" s="15"/>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="E23" s="14" t="s">
         <v>11</v>
@@ -1168,18 +1434,34 @@
       <c r="M23" s="15"/>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P23" s="15"/>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D24" s="15"/>
       <c r="E24" s="14"/>
       <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P24" s="15"/>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
       <c r="E25" s="14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P25" s="15"/>
+      <c r="R25" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="19"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="19"/>
+      <c r="Z25" s="19"/>
+      <c r="AA25" s="19"/>
+      <c r="AB25" s="19"/>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
       <c r="E26" s="14" t="s">
         <v>7</v>
@@ -1214,8 +1496,42 @@
       <c r="O26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P26" s="15"/>
+      <c r="R26" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="S26" s="19">
+        <v>2</v>
+      </c>
+      <c r="T26" s="19">
+        <v>3</v>
+      </c>
+      <c r="U26" s="19">
+        <v>4</v>
+      </c>
+      <c r="V26" s="19">
+        <v>5</v>
+      </c>
+      <c r="W26" s="19">
+        <v>7</v>
+      </c>
+      <c r="X26" s="19">
+        <v>10</v>
+      </c>
+      <c r="Y26" s="19">
+        <v>13</v>
+      </c>
+      <c r="Z26" s="19">
+        <v>15</v>
+      </c>
+      <c r="AA26" s="19">
+        <v>20</v>
+      </c>
+      <c r="AB26" s="19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
       <c r="E27" s="14" t="s">
         <v>9</v>
       </c>
@@ -1241,8 +1557,42 @@
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P27" s="15"/>
+      <c r="R27" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="S27" s="20">
+        <v>0.67618813100221598</v>
+      </c>
+      <c r="T27" s="20">
+        <v>0.73947303619797999</v>
+      </c>
+      <c r="U27" s="20">
+        <v>0.75523270130509701</v>
+      </c>
+      <c r="V27" s="20">
+        <v>0.776409751292785</v>
+      </c>
+      <c r="W27" s="20">
+        <v>0.79857178034966703</v>
+      </c>
+      <c r="X27" s="20">
+        <v>0.80768283673971897</v>
+      </c>
+      <c r="Y27" s="20">
+        <v>0.81113026348190098</v>
+      </c>
+      <c r="Z27" s="20">
+        <v>0.81383895592218602</v>
+      </c>
+      <c r="AA27" s="20">
+        <v>0.81383895592218602</v>
+      </c>
+      <c r="AB27" s="20">
+        <v>0.81482393499138095</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B28" s="15"/>
       <c r="E28" s="14" t="s">
         <v>10</v>
@@ -1269,8 +1619,9 @@
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P28" s="15"/>
+    </row>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
       <c r="E29" s="14" t="s">
         <v>11</v>
       </c>
@@ -1296,17 +1647,56 @@
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P29" s="15"/>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>
       <c r="E30" s="14"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P30" s="15"/>
+      <c r="R30" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="E31" s="14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P31" s="15"/>
+      <c r="R31" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="S31">
+        <v>2</v>
+      </c>
+      <c r="T31">
+        <v>3</v>
+      </c>
+      <c r="U31">
+        <v>4</v>
+      </c>
+      <c r="V31">
+        <v>5</v>
+      </c>
+      <c r="W31">
+        <v>7</v>
+      </c>
+      <c r="X31">
+        <v>10</v>
+      </c>
+      <c r="Y31">
+        <v>13</v>
+      </c>
+      <c r="Z31">
+        <v>15</v>
+      </c>
+      <c r="AA31">
+        <v>20</v>
+      </c>
+      <c r="AB31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B32" s="15"/>
       <c r="E32" s="14" t="s">
         <v>7</v>
@@ -1341,8 +1731,42 @@
       <c r="O32">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P32" s="15"/>
+      <c r="R32" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="S32" s="15">
+        <v>0.689401216778738</v>
+      </c>
+      <c r="T32" s="15">
+        <v>0.74479666986871496</v>
+      </c>
+      <c r="U32" s="15">
+        <v>0.76272814601344796</v>
+      </c>
+      <c r="V32" s="15">
+        <v>0.778738392571245</v>
+      </c>
+      <c r="W32" s="15">
+        <v>0.80243355747678502</v>
+      </c>
+      <c r="X32" s="15">
+        <v>0.80851745116874796</v>
+      </c>
+      <c r="Y32" s="15">
+        <v>0.81364073006724302</v>
+      </c>
+      <c r="Z32" s="15">
+        <v>0.81588216458533402</v>
+      </c>
+      <c r="AA32" s="15">
+        <v>0.81844380403458195</v>
+      </c>
+      <c r="AB32" s="15">
+        <v>0.81748318924111396</v>
+      </c>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B33" s="15"/>
       <c r="E33" s="14" t="s">
         <v>9</v>
@@ -1369,8 +1793,9 @@
       <c r="M33" s="15"/>
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P33" s="15"/>
+    </row>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
       <c r="E34" s="14" t="s">
         <v>10</v>
       </c>
@@ -1396,8 +1821,22 @@
       <c r="M34" s="15"/>
       <c r="N34" s="15"/>
       <c r="O34" s="15"/>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P34" s="15"/>
+      <c r="R34" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="19"/>
+      <c r="Y34" s="19"/>
+      <c r="Z34" s="19"/>
+      <c r="AA34" s="19"/>
+      <c r="AB34" s="19"/>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B35" s="15"/>
       <c r="E35" s="14" t="s">
         <v>11</v>
@@ -1424,29 +1863,216 @@
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P35" s="15"/>
+      <c r="R35" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="S35" s="19">
+        <v>2</v>
+      </c>
+      <c r="T35" s="19">
+        <v>3</v>
+      </c>
+      <c r="U35" s="19">
+        <v>4</v>
+      </c>
+      <c r="V35" s="19">
+        <v>5</v>
+      </c>
+      <c r="W35" s="19">
+        <v>7</v>
+      </c>
+      <c r="X35" s="19">
+        <v>10</v>
+      </c>
+      <c r="Y35" s="19">
+        <v>13</v>
+      </c>
+      <c r="Z35" s="19">
+        <v>15</v>
+      </c>
+      <c r="AA35" s="19">
+        <v>20</v>
+      </c>
+      <c r="AB35" s="19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="R36" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="S36" s="20">
+        <v>0.70562293274531396</v>
+      </c>
+      <c r="T36" s="20">
+        <v>0.76111723631018002</v>
+      </c>
+      <c r="U36" s="20">
+        <v>0.77471517824329295</v>
+      </c>
+      <c r="V36" s="20">
+        <v>0.79309077545020201</v>
+      </c>
+      <c r="W36" s="20">
+        <v>0.816244027930907</v>
+      </c>
+      <c r="X36" s="20">
+        <v>0.82102168320470403</v>
+      </c>
+      <c r="Y36" s="20">
+        <v>0.82726938625505297</v>
+      </c>
+      <c r="Z36" s="20">
+        <v>0.82800441014332904</v>
+      </c>
+      <c r="AA36" s="20">
+        <v>0.83167952958471103</v>
+      </c>
+      <c r="AB36" s="20">
+        <v>0.83094450569643497</v>
+      </c>
+    </row>
+    <row r="37" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B37" s="15"/>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P37" s="15"/>
+    </row>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="P38" s="15"/>
+      <c r="R38" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+      <c r="Y38" s="19"/>
+      <c r="Z38" s="19"/>
+      <c r="AA38" s="19"/>
+      <c r="AB38" s="19"/>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="R39" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="S39" s="19">
+        <v>2</v>
+      </c>
+      <c r="T39" s="19">
+        <v>3</v>
+      </c>
+      <c r="U39" s="19">
+        <v>4</v>
+      </c>
+      <c r="V39" s="19">
+        <v>5</v>
+      </c>
+      <c r="W39" s="19">
+        <v>7</v>
+      </c>
+      <c r="X39" s="19">
+        <v>10</v>
+      </c>
+      <c r="Y39" s="19">
+        <v>13</v>
+      </c>
+      <c r="Z39" s="19">
+        <v>15</v>
+      </c>
+      <c r="AA39" s="19">
+        <v>20</v>
+      </c>
+      <c r="AB39" s="19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B40" s="15"/>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R40" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="S40" s="20">
+        <v>0.72159921989273501</v>
+      </c>
+      <c r="T40" s="20">
+        <v>0.76986835689907296</v>
+      </c>
+      <c r="U40" s="20">
+        <v>0.78595806923451905</v>
+      </c>
+      <c r="V40" s="20">
+        <v>0.80156021452949699</v>
+      </c>
+      <c r="W40" s="20">
+        <v>0.82593856655290099</v>
+      </c>
+      <c r="X40" s="20">
+        <v>0.83130180399804898</v>
+      </c>
+      <c r="Y40" s="20">
+        <v>0.83666504144319798</v>
+      </c>
+      <c r="Z40" s="20">
+        <v>0.83715260848366602</v>
+      </c>
+      <c r="AA40" s="20">
+        <v>0.84056557776694196</v>
+      </c>
+      <c r="AB40" s="20">
+        <v>0.84300341296928305</v>
+      </c>
+    </row>
+    <row r="41" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B41" s="15"/>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R41" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="S41" s="20">
+        <v>0.71672354948805395</v>
+      </c>
+      <c r="T41" s="20">
+        <v>0.78156996587030703</v>
+      </c>
+      <c r="U41" s="20">
+        <v>0.78498293515358297</v>
+      </c>
+      <c r="V41" s="20">
+        <v>0.80497318381277405</v>
+      </c>
+      <c r="W41" s="20">
+        <v>0.82155046318868796</v>
+      </c>
+      <c r="X41" s="20">
+        <v>0.83227693807898495</v>
+      </c>
+      <c r="Y41" s="20">
+        <v>0.83520234032179397</v>
+      </c>
+      <c r="Z41" s="20">
+        <v>0.83715260848366602</v>
+      </c>
+      <c r="AA41" s="20">
+        <v>0.84056557776694196</v>
+      </c>
+      <c r="AB41" s="20">
+        <v>0.84251584592881501</v>
+      </c>
+    </row>
+    <row r="42" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B42" s="15"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B43" s="15"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B44" s="15"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B45" s="15"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B48" s="15"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
k/5 proportions graphs and tables, 10k parameters
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad1/wyniki.xlsx
+++ b/Sprawozdanie_zad1/wyniki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65C828D-DC47-4C93-85A3-936B6318FD46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3A9B17-7E88-4625-B32E-01AB151AB18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
   <si>
     <t>usa</t>
   </si>
@@ -95,10 +95,25 @@
     <t>nowe wynikimbez losowania , slowa kluczowe bez liczb i zn&lt;3</t>
   </si>
   <si>
-    <t>77 / 23</t>
+    <t>80 / 20</t>
   </si>
   <si>
-    <t>80 / 20</t>
+    <t>30/70</t>
+  </si>
+  <si>
+    <t>50/50</t>
+  </si>
+  <si>
+    <t>70/30</t>
+  </si>
+  <si>
+    <t>80/20</t>
+  </si>
+  <si>
+    <t>85/15</t>
+  </si>
+  <si>
+    <t>nie zmieniac tego na pomaranczowo bo wykresy się zmienia</t>
   </si>
 </sst>
 </file>
@@ -114,7 +129,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +145,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -248,6 +269,8 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -263,6 +286,2384 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$R$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30/70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Arkusz1!$S$10:$AB$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$S$33:$AB$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.66192548561723796</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72614372147330397</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.73813820188939605</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75873049570109297</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.77560768495913401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.779535081201571</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.78707143615327402</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.78983122810741901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79068039486254105</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.79407706188302696</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A0A0-4E4C-8C37-89CC8F4BC4BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$R$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>50/50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Arkusz1!$S$10:$AB$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$S$34:$AB$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.67141373683429695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72971369233051397</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.742471443406022</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75789942145082301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.77822281560599305</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.78742026405577803</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79261237205162405</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.793502447708055</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79735944221925503</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.79810117193294705</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A0A0-4E4C-8C37-89CC8F4BC4BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$R$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>70/30</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Arkusz1!$S$10:$AB$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$S$35:$AB$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.67618813100221598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73947303619797999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75523270130509701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.776409751292785</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79857178034966703</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80768283673971897</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.81113026348190098</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81383895592218602</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81383895592218602</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.81482393499138095</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A0A0-4E4C-8C37-89CC8F4BC4BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$R$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80/20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Arkusz1!$S$10:$AB$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$S$36:$AB$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.70562293274531396</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76111723631018002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.77471517824329295</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79309077545020201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.816244027930907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82102168320470403</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.82726938625505297</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.82800441014332904</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.83167952958471103</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.83094450569643497</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A0A0-4E4C-8C37-89CC8F4BC4BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$R$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>85/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Arkusz1!$S$10:$AB$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$S$37:$AB$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.72159921989273501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76986835689907296</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78595806923451905</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.80156021452949699</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82593856655290099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.83130180399804898</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.83666504144319798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.83715260848366602</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.84056557776694196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84300341296928305</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-A0A0-4E4C-8C37-89CC8F4BC4BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1659117232"/>
+        <c:axId val="1653040048"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1659117232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>k najbliższych sąsiadów</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1653040048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1653040048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.85000000000000009"/>
+          <c:min val="0.65000000000000013"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Skuteczność (Accuracy)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1659117232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$J$51:$J$55</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30/70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50/50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70/30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80/20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$K$51:$K$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.77949999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78739999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80769999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82099999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83130000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-49CA-4059-9AAB-C3A44F7CC152}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1761084816"/>
+        <c:axId val="1600310096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1761084816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Dane treningowe/testowe</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1600310096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1600310096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Skuteczność (Accuracy)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1761084816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{986F7276-CEC8-4D20-AB31-E115077DD9C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>138111</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Wykres 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14F32EB6-3EB5-4A6F-9583-9F02598B807D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,8 +2931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="AB36" sqref="AB36"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q75" sqref="Q75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,9 +3147,7 @@
       <c r="E7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="14" t="s">
-        <v>8</v>
-      </c>
+      <c r="R7" s="14"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E8" s="14" t="s">
@@ -784,38 +3183,9 @@
       <c r="O8">
         <v>25</v>
       </c>
-      <c r="R8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="S8">
-        <v>2</v>
-      </c>
-      <c r="T8">
-        <v>3</v>
-      </c>
-      <c r="U8">
-        <v>4</v>
-      </c>
-      <c r="V8">
-        <v>5</v>
-      </c>
-      <c r="W8">
-        <v>7</v>
-      </c>
-      <c r="X8">
-        <v>10</v>
-      </c>
-      <c r="Y8">
-        <v>13</v>
-      </c>
-      <c r="Z8">
-        <v>15</v>
-      </c>
-      <c r="AA8">
-        <v>20</v>
-      </c>
-      <c r="AB8">
-        <v>25</v>
+      <c r="R8" s="14"/>
+      <c r="U8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -852,39 +3222,19 @@
       <c r="O9" s="15">
         <v>0.79472770845384599</v>
       </c>
-      <c r="R9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="S9" s="15">
-        <v>0.65473927774564</v>
-      </c>
-      <c r="T9" s="15">
-        <v>0.73208825716882897</v>
-      </c>
-      <c r="U9" s="15">
-        <v>0.74836790347905102</v>
-      </c>
-      <c r="V9" s="15">
-        <v>0.77167176266424198</v>
-      </c>
-      <c r="W9" s="15">
-        <v>0.78456325923477399</v>
-      </c>
-      <c r="X9" s="15">
-        <v>0.79001735393769101</v>
-      </c>
-      <c r="Y9" s="15">
-        <v>0.79266176349062001</v>
-      </c>
-      <c r="Z9" s="15">
-        <v>0.79307495248326498</v>
-      </c>
-      <c r="AA9" s="15">
-        <v>0.79340550367738205</v>
-      </c>
-      <c r="AB9" s="15">
-        <v>0.79340550367738205</v>
-      </c>
+      <c r="R9" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="19"/>
+      <c r="Y9" s="19"/>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="19"/>
+      <c r="AB9" s="19"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="E10" s="14" t="s">
@@ -921,16 +3271,39 @@
         <v>0.79381869267002703</v>
       </c>
       <c r="P10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="15"/>
+      <c r="R10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="S10" s="22">
+        <v>2</v>
+      </c>
+      <c r="T10" s="22">
+        <v>3</v>
+      </c>
+      <c r="U10" s="22">
+        <v>4</v>
+      </c>
+      <c r="V10" s="22">
+        <v>5</v>
+      </c>
+      <c r="W10" s="22">
+        <v>7</v>
+      </c>
+      <c r="X10" s="22">
+        <v>10</v>
+      </c>
+      <c r="Y10" s="22">
+        <v>13</v>
+      </c>
+      <c r="Z10" s="22">
+        <v>15</v>
+      </c>
+      <c r="AA10" s="22">
+        <v>20</v>
+      </c>
+      <c r="AB10" s="22">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
@@ -970,6 +3343,39 @@
         <v>0.79522353524502098</v>
       </c>
       <c r="P11" s="15"/>
+      <c r="R11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="S11" s="20">
+        <v>0.66192548561723796</v>
+      </c>
+      <c r="T11" s="20">
+        <v>0.72614372147330397</v>
+      </c>
+      <c r="U11" s="20">
+        <v>0.73813820188939605</v>
+      </c>
+      <c r="V11" s="20">
+        <v>0.75873049570109297</v>
+      </c>
+      <c r="W11" s="20">
+        <v>0.77560768495913401</v>
+      </c>
+      <c r="X11" s="20">
+        <v>0.779535081201571</v>
+      </c>
+      <c r="Y11" s="20">
+        <v>0.78707143615327402</v>
+      </c>
+      <c r="Z11" s="20">
+        <v>0.78983122810741901</v>
+      </c>
+      <c r="AA11" s="20">
+        <v>0.79068039486254105</v>
+      </c>
+      <c r="AB11" s="20">
+        <v>0.79407706188302696</v>
+      </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
@@ -988,7 +3394,7 @@
       </c>
       <c r="P13" s="15"/>
       <c r="R13" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
@@ -1103,38 +3509,38 @@
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
-      <c r="R15" s="18" t="s">
-        <v>9</v>
+      <c r="R15" s="19" t="s">
+        <v>12</v>
       </c>
       <c r="S15" s="20">
-        <v>0.66192548561723796</v>
+        <v>0.67141373683429695</v>
       </c>
       <c r="T15" s="20">
-        <v>0.72614372147330397</v>
+        <v>0.72971369233051397</v>
       </c>
       <c r="U15" s="20">
-        <v>0.73813820188939605</v>
+        <v>0.742471443406022</v>
       </c>
       <c r="V15" s="20">
-        <v>0.75873049570109297</v>
+        <v>0.75789942145082301</v>
       </c>
       <c r="W15" s="20">
-        <v>0.77560768495913401</v>
+        <v>0.77822281560599305</v>
       </c>
       <c r="X15" s="20">
-        <v>0.779535081201571</v>
+        <v>0.78742026405577803</v>
       </c>
       <c r="Y15" s="20">
-        <v>0.78707143615327402</v>
+        <v>0.79261237205162405</v>
       </c>
       <c r="Z15" s="20">
-        <v>0.78983122810741901</v>
+        <v>0.793502447708055</v>
       </c>
       <c r="AA15" s="20">
-        <v>0.79068039486254105</v>
+        <v>0.79735944221925503</v>
       </c>
       <c r="AB15" s="20">
-        <v>0.79407706188302696</v>
+        <v>0.79810117193294705</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -1200,6 +3606,19 @@
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
+      <c r="R17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="19"/>
+      <c r="AB17" s="19"/>
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B18" s="15">
@@ -1209,6 +3628,39 @@
       <c r="D18" s="15"/>
       <c r="E18" s="14"/>
       <c r="P18" s="15"/>
+      <c r="R18" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="S18" s="19">
+        <v>2</v>
+      </c>
+      <c r="T18" s="19">
+        <v>3</v>
+      </c>
+      <c r="U18" s="19">
+        <v>4</v>
+      </c>
+      <c r="V18" s="19">
+        <v>5</v>
+      </c>
+      <c r="W18" s="19">
+        <v>7</v>
+      </c>
+      <c r="X18" s="19">
+        <v>10</v>
+      </c>
+      <c r="Y18" s="19">
+        <v>13</v>
+      </c>
+      <c r="Z18" s="19">
+        <v>15</v>
+      </c>
+      <c r="AA18" s="19">
+        <v>20</v>
+      </c>
+      <c r="AB18" s="19">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
@@ -1221,18 +3673,38 @@
       </c>
       <c r="P19" s="15"/>
       <c r="R19" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
-      <c r="W19" s="19"/>
-      <c r="X19" s="19"/>
-      <c r="Y19" s="19"/>
-      <c r="Z19" s="19"/>
-      <c r="AA19" s="19"/>
-      <c r="AB19" s="19"/>
+        <v>9</v>
+      </c>
+      <c r="S19" s="20">
+        <v>0.67618813100221598</v>
+      </c>
+      <c r="T19" s="20">
+        <v>0.73947303619797999</v>
+      </c>
+      <c r="U19" s="20">
+        <v>0.75523270130509701</v>
+      </c>
+      <c r="V19" s="20">
+        <v>0.776409751292785</v>
+      </c>
+      <c r="W19" s="20">
+        <v>0.79857178034966703</v>
+      </c>
+      <c r="X19" s="20">
+        <v>0.80768283673971897</v>
+      </c>
+      <c r="Y19" s="20">
+        <v>0.81113026348190098</v>
+      </c>
+      <c r="Z19" s="20">
+        <v>0.81383895592218602</v>
+      </c>
+      <c r="AA19" s="20">
+        <v>0.81383895592218602</v>
+      </c>
+      <c r="AB19" s="20">
+        <v>0.81482393499138095</v>
+      </c>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B20" s="15">
@@ -1274,39 +3746,6 @@
         <v>25</v>
       </c>
       <c r="P20" s="15"/>
-      <c r="R20" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="S20" s="19">
-        <v>2</v>
-      </c>
-      <c r="T20" s="19">
-        <v>3</v>
-      </c>
-      <c r="U20" s="19">
-        <v>4</v>
-      </c>
-      <c r="V20" s="19">
-        <v>5</v>
-      </c>
-      <c r="W20" s="19">
-        <v>7</v>
-      </c>
-      <c r="X20" s="19">
-        <v>10</v>
-      </c>
-      <c r="Y20" s="19">
-        <v>13</v>
-      </c>
-      <c r="Z20" s="19">
-        <v>15</v>
-      </c>
-      <c r="AA20" s="19">
-        <v>20</v>
-      </c>
-      <c r="AB20" s="19">
-        <v>25</v>
-      </c>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
@@ -1340,39 +3779,19 @@
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
       <c r="P21" s="15"/>
-      <c r="R21" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="S21" s="20">
-        <v>0.67141373683429695</v>
-      </c>
-      <c r="T21" s="20">
-        <v>0.72971369233051397</v>
-      </c>
-      <c r="U21" s="20">
-        <v>0.742471443406022</v>
-      </c>
-      <c r="V21" s="20">
-        <v>0.75789942145082301</v>
-      </c>
-      <c r="W21" s="20">
-        <v>0.77822281560599305</v>
-      </c>
-      <c r="X21" s="20">
-        <v>0.78742026405577803</v>
-      </c>
-      <c r="Y21" s="20">
-        <v>0.79261237205162405</v>
-      </c>
-      <c r="Z21" s="20">
-        <v>0.793502447708055</v>
-      </c>
-      <c r="AA21" s="20">
-        <v>0.79735944221925503</v>
-      </c>
-      <c r="AB21" s="20">
-        <v>0.79810117193294705</v>
-      </c>
+      <c r="R21" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="19"/>
+      <c r="AA21" s="19"/>
+      <c r="AB21" s="19"/>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B22" s="15">
@@ -1406,6 +3825,39 @@
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
+      <c r="R22" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="S22" s="19">
+        <v>2</v>
+      </c>
+      <c r="T22" s="19">
+        <v>3</v>
+      </c>
+      <c r="U22" s="19">
+        <v>4</v>
+      </c>
+      <c r="V22" s="19">
+        <v>5</v>
+      </c>
+      <c r="W22" s="19">
+        <v>7</v>
+      </c>
+      <c r="X22" s="19">
+        <v>10</v>
+      </c>
+      <c r="Y22" s="19">
+        <v>13</v>
+      </c>
+      <c r="Z22" s="19">
+        <v>15</v>
+      </c>
+      <c r="AA22" s="19">
+        <v>20</v>
+      </c>
+      <c r="AB22" s="19">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
@@ -1435,6 +3887,39 @@
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
+      <c r="R23" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="S23" s="20">
+        <v>0.70562293274531396</v>
+      </c>
+      <c r="T23" s="20">
+        <v>0.76111723631018002</v>
+      </c>
+      <c r="U23" s="20">
+        <v>0.77471517824329295</v>
+      </c>
+      <c r="V23" s="20">
+        <v>0.79309077545020201</v>
+      </c>
+      <c r="W23" s="20">
+        <v>0.816244027930907</v>
+      </c>
+      <c r="X23" s="20">
+        <v>0.82102168320470403</v>
+      </c>
+      <c r="Y23" s="20">
+        <v>0.82726938625505297</v>
+      </c>
+      <c r="Z23" s="20">
+        <v>0.82800441014332904</v>
+      </c>
+      <c r="AA23" s="20">
+        <v>0.83167952958471103</v>
+      </c>
+      <c r="AB23" s="20">
+        <v>0.83094450569643497</v>
+      </c>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D24" s="15"/>
@@ -1448,7 +3933,7 @@
       </c>
       <c r="P25" s="15"/>
       <c r="R25" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S25" s="19"/>
       <c r="T25" s="19"/>
@@ -1562,34 +4047,34 @@
         <v>9</v>
       </c>
       <c r="S27" s="20">
-        <v>0.67618813100221598</v>
+        <v>0.72159921989273501</v>
       </c>
       <c r="T27" s="20">
-        <v>0.73947303619797999</v>
+        <v>0.76986835689907296</v>
       </c>
       <c r="U27" s="20">
-        <v>0.75523270130509701</v>
+        <v>0.78595806923451905</v>
       </c>
       <c r="V27" s="20">
-        <v>0.776409751292785</v>
+        <v>0.80156021452949699</v>
       </c>
       <c r="W27" s="20">
-        <v>0.79857178034966703</v>
+        <v>0.82593856655290099</v>
       </c>
       <c r="X27" s="20">
-        <v>0.80768283673971897</v>
+        <v>0.83130180399804898</v>
       </c>
       <c r="Y27" s="20">
-        <v>0.81113026348190098</v>
+        <v>0.83666504144319798</v>
       </c>
       <c r="Z27" s="20">
-        <v>0.81383895592218602</v>
+        <v>0.83715260848366602</v>
       </c>
       <c r="AA27" s="20">
-        <v>0.81383895592218602</v>
+        <v>0.84056557776694196</v>
       </c>
       <c r="AB27" s="20">
-        <v>0.81482393499138095</v>
+        <v>0.84300341296928305</v>
       </c>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.25">
@@ -1620,6 +4105,17 @@
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="21"/>
+      <c r="U28" s="21"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="21"/>
+      <c r="X28" s="21"/>
+      <c r="Y28" s="21"/>
+      <c r="Z28" s="21"/>
+      <c r="AA28" s="21"/>
+      <c r="AB28" s="21"/>
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.25">
       <c r="E29" s="14" t="s">
@@ -1653,48 +4149,14 @@
       <c r="B30" s="15"/>
       <c r="E30" s="14"/>
       <c r="P30" s="15"/>
-      <c r="R30" s="14" t="s">
-        <v>20</v>
-      </c>
+      <c r="R30" s="14"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="E31" s="14" t="s">
         <v>18</v>
       </c>
       <c r="P31" s="15"/>
-      <c r="R31" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="S31">
-        <v>2</v>
-      </c>
-      <c r="T31">
-        <v>3</v>
-      </c>
-      <c r="U31">
-        <v>4</v>
-      </c>
-      <c r="V31">
-        <v>5</v>
-      </c>
-      <c r="W31">
-        <v>7</v>
-      </c>
-      <c r="X31">
-        <v>10</v>
-      </c>
-      <c r="Y31">
-        <v>13</v>
-      </c>
-      <c r="Z31">
-        <v>15</v>
-      </c>
-      <c r="AA31">
-        <v>20</v>
-      </c>
-      <c r="AB31">
-        <v>25</v>
-      </c>
+      <c r="R31" s="14"/>
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B32" s="15"/>
@@ -1732,39 +4194,17 @@
         <v>25</v>
       </c>
       <c r="P32" s="15"/>
-      <c r="R32" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="S32" s="15">
-        <v>0.689401216778738</v>
-      </c>
-      <c r="T32" s="15">
-        <v>0.74479666986871496</v>
-      </c>
-      <c r="U32" s="15">
-        <v>0.76272814601344796</v>
-      </c>
-      <c r="V32" s="15">
-        <v>0.778738392571245</v>
-      </c>
-      <c r="W32" s="15">
-        <v>0.80243355747678502</v>
-      </c>
-      <c r="X32" s="15">
-        <v>0.80851745116874796</v>
-      </c>
-      <c r="Y32" s="15">
-        <v>0.81364073006724302</v>
-      </c>
-      <c r="Z32" s="15">
-        <v>0.81588216458533402</v>
-      </c>
-      <c r="AA32" s="15">
-        <v>0.81844380403458195</v>
-      </c>
-      <c r="AB32" s="15">
-        <v>0.81748318924111396</v>
-      </c>
+      <c r="R32" s="14"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="15"/>
+      <c r="V32" s="15"/>
+      <c r="W32" s="15"/>
+      <c r="X32" s="15"/>
+      <c r="Y32" s="15"/>
+      <c r="Z32" s="15"/>
+      <c r="AA32" s="15"/>
+      <c r="AB32" s="15"/>
     </row>
     <row r="33" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B33" s="15"/>
@@ -1794,6 +4234,39 @@
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
+      <c r="R33" t="s">
+        <v>21</v>
+      </c>
+      <c r="S33" s="20">
+        <v>0.66192548561723796</v>
+      </c>
+      <c r="T33" s="20">
+        <v>0.72614372147330397</v>
+      </c>
+      <c r="U33" s="20">
+        <v>0.73813820188939605</v>
+      </c>
+      <c r="V33" s="20">
+        <v>0.75873049570109297</v>
+      </c>
+      <c r="W33" s="20">
+        <v>0.77560768495913401</v>
+      </c>
+      <c r="X33" s="20">
+        <v>0.779535081201571</v>
+      </c>
+      <c r="Y33" s="20">
+        <v>0.78707143615327402</v>
+      </c>
+      <c r="Z33" s="20">
+        <v>0.78983122810741901</v>
+      </c>
+      <c r="AA33" s="20">
+        <v>0.79068039486254105</v>
+      </c>
+      <c r="AB33" s="20">
+        <v>0.79407706188302696</v>
+      </c>
     </row>
     <row r="34" spans="2:28" x14ac:dyDescent="0.25">
       <c r="E34" s="14" t="s">
@@ -1822,19 +4295,39 @@
       <c r="N34" s="15"/>
       <c r="O34" s="15"/>
       <c r="P34" s="15"/>
-      <c r="R34" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-      <c r="W34" s="19"/>
-      <c r="X34" s="19"/>
-      <c r="Y34" s="19"/>
-      <c r="Z34" s="19"/>
-      <c r="AA34" s="19"/>
-      <c r="AB34" s="19"/>
+      <c r="R34" t="s">
+        <v>22</v>
+      </c>
+      <c r="S34" s="20">
+        <v>0.67141373683429695</v>
+      </c>
+      <c r="T34" s="20">
+        <v>0.72971369233051397</v>
+      </c>
+      <c r="U34" s="20">
+        <v>0.742471443406022</v>
+      </c>
+      <c r="V34" s="20">
+        <v>0.75789942145082301</v>
+      </c>
+      <c r="W34" s="20">
+        <v>0.77822281560599305</v>
+      </c>
+      <c r="X34" s="20">
+        <v>0.78742026405577803</v>
+      </c>
+      <c r="Y34" s="20">
+        <v>0.79261237205162405</v>
+      </c>
+      <c r="Z34" s="20">
+        <v>0.793502447708055</v>
+      </c>
+      <c r="AA34" s="20">
+        <v>0.79735944221925503</v>
+      </c>
+      <c r="AB34" s="20">
+        <v>0.79810117193294705</v>
+      </c>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B35" s="15"/>
@@ -1864,43 +4357,43 @@
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
       <c r="P35" s="15"/>
-      <c r="R35" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="S35" s="19">
-        <v>2</v>
-      </c>
-      <c r="T35" s="19">
-        <v>3</v>
-      </c>
-      <c r="U35" s="19">
-        <v>4</v>
-      </c>
-      <c r="V35" s="19">
-        <v>5</v>
-      </c>
-      <c r="W35" s="19">
-        <v>7</v>
-      </c>
-      <c r="X35" s="19">
-        <v>10</v>
-      </c>
-      <c r="Y35" s="19">
-        <v>13</v>
-      </c>
-      <c r="Z35" s="19">
-        <v>15</v>
-      </c>
-      <c r="AA35" s="19">
-        <v>20</v>
-      </c>
-      <c r="AB35" s="19">
-        <v>25</v>
+      <c r="R35" t="s">
+        <v>23</v>
+      </c>
+      <c r="S35" s="20">
+        <v>0.67618813100221598</v>
+      </c>
+      <c r="T35" s="20">
+        <v>0.73947303619797999</v>
+      </c>
+      <c r="U35" s="20">
+        <v>0.75523270130509701</v>
+      </c>
+      <c r="V35" s="20">
+        <v>0.776409751292785</v>
+      </c>
+      <c r="W35" s="20">
+        <v>0.79857178034966703</v>
+      </c>
+      <c r="X35" s="20">
+        <v>0.80768283673971897</v>
+      </c>
+      <c r="Y35" s="20">
+        <v>0.81113026348190098</v>
+      </c>
+      <c r="Z35" s="20">
+        <v>0.81383895592218602</v>
+      </c>
+      <c r="AA35" s="20">
+        <v>0.81383895592218602</v>
+      </c>
+      <c r="AB35" s="20">
+        <v>0.81482393499138095</v>
       </c>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="R36" s="18" t="s">
-        <v>9</v>
+      <c r="R36" t="s">
+        <v>24</v>
       </c>
       <c r="S36" s="20">
         <v>0.70562293274531396</v>
@@ -1936,129 +4429,48 @@
     <row r="37" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B37" s="15"/>
       <c r="P37" s="15"/>
+      <c r="R37" t="s">
+        <v>25</v>
+      </c>
+      <c r="S37" s="20">
+        <v>0.72159921989273501</v>
+      </c>
+      <c r="T37" s="20">
+        <v>0.76986835689907296</v>
+      </c>
+      <c r="U37" s="20">
+        <v>0.78595806923451905</v>
+      </c>
+      <c r="V37" s="20">
+        <v>0.80156021452949699</v>
+      </c>
+      <c r="W37" s="20">
+        <v>0.82593856655290099</v>
+      </c>
+      <c r="X37" s="20">
+        <v>0.83130180399804898</v>
+      </c>
+      <c r="Y37" s="20">
+        <v>0.83666504144319798</v>
+      </c>
+      <c r="Z37" s="20">
+        <v>0.83715260848366602</v>
+      </c>
+      <c r="AA37" s="20">
+        <v>0.84056557776694196</v>
+      </c>
+      <c r="AB37" s="20">
+        <v>0.84300341296928305</v>
+      </c>
     </row>
     <row r="38" spans="2:28" x14ac:dyDescent="0.25">
       <c r="P38" s="15"/>
-      <c r="R38" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="19"/>
-      <c r="Y38" s="19"/>
-      <c r="Z38" s="19"/>
-      <c r="AA38" s="19"/>
-      <c r="AB38" s="19"/>
-    </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="R39" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="S39" s="19">
-        <v>2</v>
-      </c>
-      <c r="T39" s="19">
-        <v>3</v>
-      </c>
-      <c r="U39" s="19">
-        <v>4</v>
-      </c>
-      <c r="V39" s="19">
-        <v>5</v>
-      </c>
-      <c r="W39" s="19">
-        <v>7</v>
-      </c>
-      <c r="X39" s="19">
-        <v>10</v>
-      </c>
-      <c r="Y39" s="19">
-        <v>13</v>
-      </c>
-      <c r="Z39" s="19">
-        <v>15</v>
-      </c>
-      <c r="AA39" s="19">
-        <v>20</v>
-      </c>
-      <c r="AB39" s="19">
-        <v>25</v>
-      </c>
     </row>
     <row r="40" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B40" s="15"/>
-      <c r="R40" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="S40" s="20">
-        <v>0.72159921989273501</v>
-      </c>
-      <c r="T40" s="20">
-        <v>0.76986835689907296</v>
-      </c>
-      <c r="U40" s="20">
-        <v>0.78595806923451905</v>
-      </c>
-      <c r="V40" s="20">
-        <v>0.80156021452949699</v>
-      </c>
-      <c r="W40" s="20">
-        <v>0.82593856655290099</v>
-      </c>
-      <c r="X40" s="20">
-        <v>0.83130180399804898</v>
-      </c>
-      <c r="Y40" s="20">
-        <v>0.83666504144319798</v>
-      </c>
-      <c r="Z40" s="20">
-        <v>0.83715260848366602</v>
-      </c>
-      <c r="AA40" s="20">
-        <v>0.84056557776694196</v>
-      </c>
-      <c r="AB40" s="20">
-        <v>0.84300341296928305</v>
-      </c>
     </row>
     <row r="41" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B41" s="15"/>
-      <c r="R41" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="S41" s="20">
-        <v>0.71672354948805395</v>
-      </c>
-      <c r="T41" s="20">
-        <v>0.78156996587030703</v>
-      </c>
-      <c r="U41" s="20">
-        <v>0.78498293515358297</v>
-      </c>
-      <c r="V41" s="20">
-        <v>0.80497318381277405</v>
-      </c>
-      <c r="W41" s="20">
-        <v>0.82155046318868796</v>
-      </c>
-      <c r="X41" s="20">
-        <v>0.83227693807898495</v>
-      </c>
-      <c r="Y41" s="20">
-        <v>0.83520234032179397</v>
-      </c>
-      <c r="Z41" s="20">
-        <v>0.83715260848366602</v>
-      </c>
-      <c r="AA41" s="20">
-        <v>0.84056557776694196</v>
-      </c>
-      <c r="AB41" s="20">
-        <v>0.84251584592881501</v>
-      </c>
     </row>
     <row r="42" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B42" s="15"/>
@@ -2075,25 +4487,62 @@
     <row r="48" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B48" s="15"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="15"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>21</v>
+      </c>
+      <c r="K51" s="15">
+        <v>0.77949999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="15"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>22</v>
+      </c>
+      <c r="K52" s="15">
+        <v>0.78739999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" s="15">
+        <v>0.80769999999999997</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="15"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>24</v>
+      </c>
+      <c r="K54" s="15">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>25</v>
+      </c>
+      <c r="K55" s="15">
+        <v>0.83130000000000004</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" s="15"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" s="15"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More graphs and tables
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad1/wyniki.xlsx
+++ b/Sprawozdanie_zad1/wyniki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3A9B17-7E88-4625-B32E-01AB151AB18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1581484C-444F-4C6F-89CD-7FBB574210E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
   <si>
     <t>usa</t>
   </si>
@@ -74,12 +74,6 @@
     <t>Euclides</t>
   </si>
   <si>
-    <t>Chebyshew</t>
-  </si>
-  <si>
-    <t>Manhattan</t>
-  </si>
-  <si>
     <t>30 / 70</t>
   </si>
   <si>
@@ -113,7 +107,16 @@
     <t>85/15</t>
   </si>
   <si>
-    <t>nie zmieniac tego na pomaranczowo bo wykresy się zmienia</t>
+    <t>euclides</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>nie zmieniac tego ciemniejszego bo wykresy się zmienia</t>
+  </si>
+  <si>
+    <t>k = 7</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,13 +147,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFE3DE00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -264,19 +261,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE3DE00"/>
+      <color rgb="FFF9FF01"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1537,6 +1541,826 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$R$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>euclidean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Arkusz1!$S$18:$AB$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$S$19:$AB$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.67618813100221598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73947303619797999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75523270130509701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.776409751292785</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79857178034966703</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80768283673971897</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.81113026348190098</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81383895592218602</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81383895592218602</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.81482393499138095</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2030-4D5A-B2EC-D48CE23C8A4A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1846716239"/>
+        <c:axId val="1834833119"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1846716239"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>k najbliższych sąsiadów</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1834833119"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1834833119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.65000000000000013"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Skuteczność (Accuracy)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1846716239"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1200" baseline="0"/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$AG$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>euclides</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$AF$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$AG$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.77822281560599305</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2129-4F54-95D1-E531A25BD1C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$AH$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>chebyshew</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$AF$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$AH$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.78178311823171598</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2129-4F54-95D1-E531A25BD1C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$AI$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>manhattan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$AF$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$AI$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.77718439400682404</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2129-4F54-95D1-E531A25BD1C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1984431295"/>
+        <c:axId val="1845564703"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1984431295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1845564703"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1845564703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.78600000000000003"/>
+          <c:min val="0.77600000000000002"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+                  <a:t>Skuteczność (Accuracy)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1984431295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1617,6 +2441,83 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2585,6 +3486,1012 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx2"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2658,6 +4565,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>122465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>326572</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>176894</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{133A8E97-E8E6-4615-BA1D-D847DEC8AB48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Wykres 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B0B1887-97A8-44CA-8AA4-4138390E5B40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2929,10 +4908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB61"/>
+  <dimension ref="A1:AI61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q75" sqref="Q75"/>
+    <sheetView tabSelected="1" topLeftCell="R7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2940,9 +4919,10 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="18" max="18" width="11.85546875" customWidth="1"/>
+    <col min="32" max="32" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5">
         <v>322</v>
       </c>
@@ -2950,7 +4930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>10685</v>
       </c>
@@ -3025,7 +5005,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>251</v>
       </c>
@@ -3116,7 +5096,7 @@
         <v>13440</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>905</v>
       </c>
@@ -3124,7 +5104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>812</v>
       </c>
@@ -3132,7 +5112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>466</v>
       </c>
@@ -3140,16 +5120,16 @@
         <v>2</v>
       </c>
       <c r="R6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E7" s="14" t="s">
         <v>8</v>
       </c>
       <c r="R7" s="14"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E8" s="14" t="s">
         <v>7</v>
       </c>
@@ -3188,7 +5168,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E9" s="14" t="s">
         <v>9</v>
       </c>
@@ -3222,21 +5202,21 @@
       <c r="O9" s="15">
         <v>0.79472770845384599</v>
       </c>
-      <c r="R9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="19"/>
-      <c r="X9" s="19"/>
-      <c r="Y9" s="19"/>
-      <c r="Z9" s="19"/>
-      <c r="AA9" s="19"/>
-      <c r="AB9" s="19"/>
+      <c r="R9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="18"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E10" s="14" t="s">
         <v>10</v>
       </c>
@@ -3271,41 +5251,44 @@
         <v>0.79381869267002703</v>
       </c>
       <c r="P10" s="15"/>
-      <c r="R10" s="18" t="s">
+      <c r="R10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="S10" s="22">
+      <c r="S10" s="21">
         <v>2</v>
       </c>
-      <c r="T10" s="22">
+      <c r="T10" s="21">
         <v>3</v>
       </c>
-      <c r="U10" s="22">
+      <c r="U10" s="21">
         <v>4</v>
       </c>
-      <c r="V10" s="22">
+      <c r="V10" s="21">
         <v>5</v>
       </c>
-      <c r="W10" s="22">
+      <c r="W10" s="21">
         <v>7</v>
       </c>
-      <c r="X10" s="22">
+      <c r="X10" s="21">
         <v>10</v>
       </c>
-      <c r="Y10" s="22">
+      <c r="Y10" s="21">
         <v>13</v>
       </c>
-      <c r="Z10" s="22">
+      <c r="Z10" s="21">
         <v>15</v>
       </c>
-      <c r="AA10" s="22">
+      <c r="AA10" s="21">
         <v>20</v>
       </c>
-      <c r="AB10" s="22">
+      <c r="AB10" s="21">
         <v>25</v>
       </c>
+      <c r="AF10" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -3343,71 +5326,101 @@
         <v>0.79522353524502098</v>
       </c>
       <c r="P11" s="15"/>
-      <c r="R11" s="18" t="s">
+      <c r="R11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="S11" s="20">
+      <c r="S11" s="19">
         <v>0.66192548561723796</v>
       </c>
-      <c r="T11" s="20">
+      <c r="T11" s="19">
         <v>0.72614372147330397</v>
       </c>
-      <c r="U11" s="20">
+      <c r="U11" s="19">
         <v>0.73813820188939605</v>
       </c>
-      <c r="V11" s="20">
+      <c r="V11" s="19">
         <v>0.75873049570109297</v>
       </c>
-      <c r="W11" s="20">
+      <c r="W11" s="19">
         <v>0.77560768495913401</v>
       </c>
-      <c r="X11" s="20">
+      <c r="X11" s="19">
         <v>0.779535081201571</v>
       </c>
-      <c r="Y11" s="20">
+      <c r="Y11" s="19">
         <v>0.78707143615327402</v>
       </c>
-      <c r="Z11" s="20">
+      <c r="Z11" s="19">
         <v>0.78983122810741901</v>
       </c>
-      <c r="AA11" s="20">
+      <c r="AA11" s="19">
         <v>0.79068039486254105</v>
       </c>
-      <c r="AB11" s="20">
+      <c r="AB11" s="19">
         <v>0.79407706188302696</v>
       </c>
+      <c r="AF11" s="21"/>
+      <c r="AG11" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI11" s="21" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="H12" s="15"/>
       <c r="P12" s="15"/>
+      <c r="AE12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF12" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG12" s="22">
+        <v>0.77822281560599305</v>
+      </c>
+      <c r="AH12" s="22">
+        <v>0.78178311823171598</v>
+      </c>
+      <c r="AI12" s="22">
+        <v>0.77718439400682404</v>
+      </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="P13" s="15"/>
-      <c r="R13" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19"/>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="19"/>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="19"/>
+      <c r="R13" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="18"/>
+      <c r="AA13" s="18"/>
+      <c r="AB13" s="18"/>
+      <c r="AF13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG13" s="15"/>
+      <c r="AI13" s="15"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -3445,41 +5458,46 @@
         <v>25</v>
       </c>
       <c r="P14" s="15"/>
-      <c r="R14" s="18" t="s">
+      <c r="R14" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="S14" s="19">
+      <c r="S14" s="18">
         <v>2</v>
       </c>
-      <c r="T14" s="19">
+      <c r="T14" s="18">
         <v>3</v>
       </c>
-      <c r="U14" s="19">
+      <c r="U14" s="18">
         <v>4</v>
       </c>
-      <c r="V14" s="19">
+      <c r="V14" s="18">
         <v>5</v>
       </c>
-      <c r="W14" s="19">
+      <c r="W14" s="18">
         <v>7</v>
       </c>
-      <c r="X14" s="19">
+      <c r="X14" s="18">
         <v>10</v>
       </c>
-      <c r="Y14" s="19">
+      <c r="Y14" s="18">
         <v>13</v>
       </c>
-      <c r="Z14" s="19">
+      <c r="Z14" s="18">
         <v>15</v>
       </c>
-      <c r="AA14" s="19">
+      <c r="AA14" s="18">
         <v>20</v>
       </c>
-      <c r="AB14" s="19">
+      <c r="AB14" s="18">
         <v>25</v>
       </c>
+      <c r="AF14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG14" s="15"/>
+      <c r="AI14" s="15"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -3509,44 +5527,47 @@
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
-      <c r="R15" s="19" t="s">
+      <c r="R15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="S15" s="20">
+      <c r="S15" s="19">
         <v>0.67141373683429695</v>
       </c>
-      <c r="T15" s="20">
+      <c r="T15" s="19">
         <v>0.72971369233051397</v>
       </c>
-      <c r="U15" s="20">
+      <c r="U15" s="19">
         <v>0.742471443406022</v>
       </c>
-      <c r="V15" s="20">
+      <c r="V15" s="19">
         <v>0.75789942145082301</v>
       </c>
-      <c r="W15" s="20">
+      <c r="W15" s="19">
         <v>0.77822281560599305</v>
       </c>
-      <c r="X15" s="20">
+      <c r="X15" s="19">
         <v>0.78742026405577803</v>
       </c>
-      <c r="Y15" s="20">
+      <c r="Y15" s="19">
         <v>0.79261237205162405</v>
       </c>
-      <c r="Z15" s="20">
+      <c r="Z15" s="19">
         <v>0.793502447708055</v>
       </c>
-      <c r="AA15" s="20">
+      <c r="AA15" s="19">
         <v>0.79735944221925503</v>
       </c>
-      <c r="AB15" s="20">
+      <c r="AB15" s="19">
         <v>0.79810117193294705</v>
       </c>
+      <c r="AF15" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
-      <c r="D16" s="17"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="14" t="s">
         <v>10</v>
       </c>
@@ -3573,11 +5594,12 @@
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
+      <c r="AF16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
-        <v>12</v>
-      </c>
+      <c r="B17" s="16"/>
       <c r="C17" s="14"/>
       <c r="D17" s="15"/>
       <c r="E17" s="14" t="s">
@@ -3606,110 +5628,104 @@
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
-      <c r="R17" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
-      <c r="W17" s="19"/>
-      <c r="X17" s="19"/>
-      <c r="Y17" s="19"/>
-      <c r="Z17" s="19"/>
-      <c r="AA17" s="19"/>
-      <c r="AB17" s="19"/>
+      <c r="R17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="18"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="18"/>
+      <c r="X17" s="18"/>
+      <c r="Y17" s="18"/>
+      <c r="Z17" s="18"/>
+      <c r="AA17" s="18"/>
+      <c r="AB17" s="18"/>
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B18" s="15">
-        <v>0.77279375914188198</v>
-      </c>
+      <c r="B18" s="15"/>
       <c r="C18" s="14"/>
       <c r="D18" s="15"/>
       <c r="E18" s="14"/>
       <c r="P18" s="15"/>
-      <c r="R18" s="18" t="s">
+      <c r="R18" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="S18" s="19">
+      <c r="S18" s="21">
         <v>2</v>
       </c>
-      <c r="T18" s="19">
+      <c r="T18" s="21">
         <v>3</v>
       </c>
-      <c r="U18" s="19">
+      <c r="U18" s="21">
         <v>4</v>
       </c>
-      <c r="V18" s="19">
+      <c r="V18" s="21">
         <v>5</v>
       </c>
-      <c r="W18" s="19">
+      <c r="W18" s="21">
         <v>7</v>
       </c>
-      <c r="X18" s="19">
+      <c r="X18" s="21">
         <v>10</v>
       </c>
-      <c r="Y18" s="19">
+      <c r="Y18" s="21">
         <v>13</v>
       </c>
-      <c r="Z18" s="19">
+      <c r="Z18" s="21">
         <v>15</v>
       </c>
-      <c r="AA18" s="19">
+      <c r="AA18" s="21">
         <v>20</v>
       </c>
-      <c r="AB18" s="19">
+      <c r="AB18" s="21">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
-        <v>13</v>
-      </c>
+      <c r="B19" s="15"/>
       <c r="C19" s="14"/>
       <c r="D19" s="15"/>
       <c r="E19" s="14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="P19" s="15"/>
-      <c r="R19" s="18" t="s">
+      <c r="R19" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="S19" s="20">
+      <c r="S19" s="22">
         <v>0.67618813100221598</v>
       </c>
-      <c r="T19" s="20">
+      <c r="T19" s="22">
         <v>0.73947303619797999</v>
       </c>
-      <c r="U19" s="20">
+      <c r="U19" s="22">
         <v>0.75523270130509701</v>
       </c>
-      <c r="V19" s="20">
+      <c r="V19" s="22">
         <v>0.776409751292785</v>
       </c>
-      <c r="W19" s="20">
+      <c r="W19" s="22">
         <v>0.79857178034966703</v>
       </c>
-      <c r="X19" s="20">
+      <c r="X19" s="22">
         <v>0.80768283673971897</v>
       </c>
-      <c r="Y19" s="20">
+      <c r="Y19" s="22">
         <v>0.81113026348190098</v>
       </c>
-      <c r="Z19" s="20">
+      <c r="Z19" s="22">
         <v>0.81383895592218602</v>
       </c>
-      <c r="AA19" s="20">
+      <c r="AA19" s="22">
         <v>0.81383895592218602</v>
       </c>
-      <c r="AB19" s="20">
+      <c r="AB19" s="22">
         <v>0.81482393499138095</v>
       </c>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B20" s="15">
-        <v>0.79180887372013598</v>
-      </c>
+      <c r="B20" s="15"/>
       <c r="C20" s="14"/>
       <c r="D20" s="15"/>
       <c r="E20" s="14" t="s">
@@ -3748,9 +5764,7 @@
       <c r="P20" s="15"/>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B21" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="B21" s="15"/>
       <c r="C21" s="14"/>
       <c r="D21" s="15"/>
       <c r="E21" s="14" t="s">
@@ -3779,24 +5793,22 @@
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
       <c r="P21" s="15"/>
-      <c r="R21" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="19"/>
-      <c r="X21" s="19"/>
-      <c r="Y21" s="19"/>
-      <c r="Z21" s="19"/>
-      <c r="AA21" s="19"/>
-      <c r="AB21" s="19"/>
+      <c r="R21" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="S21" s="18"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+      <c r="W21" s="18"/>
+      <c r="X21" s="18"/>
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="18"/>
+      <c r="AA21" s="18"/>
+      <c r="AB21" s="18"/>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B22" s="15">
-        <v>0.79229644076060401</v>
-      </c>
+      <c r="B22" s="15"/>
       <c r="C22" s="14"/>
       <c r="D22" s="15"/>
       <c r="E22" s="14" t="s">
@@ -3825,37 +5837,37 @@
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
-      <c r="R22" s="18" t="s">
+      <c r="R22" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="S22" s="19">
+      <c r="S22" s="18">
         <v>2</v>
       </c>
-      <c r="T22" s="19">
+      <c r="T22" s="18">
         <v>3</v>
       </c>
-      <c r="U22" s="19">
+      <c r="U22" s="18">
         <v>4</v>
       </c>
-      <c r="V22" s="19">
+      <c r="V22" s="18">
         <v>5</v>
       </c>
-      <c r="W22" s="19">
+      <c r="W22" s="18">
         <v>7</v>
       </c>
-      <c r="X22" s="19">
+      <c r="X22" s="18">
         <v>10</v>
       </c>
-      <c r="Y22" s="19">
+      <c r="Y22" s="18">
         <v>13</v>
       </c>
-      <c r="Z22" s="19">
+      <c r="Z22" s="18">
         <v>15</v>
       </c>
-      <c r="AA22" s="19">
+      <c r="AA22" s="18">
         <v>20</v>
       </c>
-      <c r="AB22" s="19">
+      <c r="AB22" s="18">
         <v>25</v>
       </c>
     </row>
@@ -3887,37 +5899,37 @@
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
-      <c r="R23" s="18" t="s">
+      <c r="R23" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="S23" s="20">
+      <c r="S23" s="19">
         <v>0.70562293274531396</v>
       </c>
-      <c r="T23" s="20">
+      <c r="T23" s="19">
         <v>0.76111723631018002</v>
       </c>
-      <c r="U23" s="20">
+      <c r="U23" s="19">
         <v>0.77471517824329295</v>
       </c>
-      <c r="V23" s="20">
+      <c r="V23" s="19">
         <v>0.79309077545020201</v>
       </c>
-      <c r="W23" s="20">
+      <c r="W23" s="19">
         <v>0.816244027930907</v>
       </c>
-      <c r="X23" s="20">
+      <c r="X23" s="19">
         <v>0.82102168320470403</v>
       </c>
-      <c r="Y23" s="20">
+      <c r="Y23" s="19">
         <v>0.82726938625505297</v>
       </c>
-      <c r="Z23" s="20">
+      <c r="Z23" s="19">
         <v>0.82800441014332904</v>
       </c>
-      <c r="AA23" s="20">
+      <c r="AA23" s="19">
         <v>0.83167952958471103</v>
       </c>
-      <c r="AB23" s="20">
+      <c r="AB23" s="19">
         <v>0.83094450569643497</v>
       </c>
     </row>
@@ -3929,22 +5941,22 @@
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.25">
       <c r="E25" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P25" s="15"/>
-      <c r="R25" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19"/>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="19"/>
-      <c r="Z25" s="19"/>
-      <c r="AA25" s="19"/>
-      <c r="AB25" s="19"/>
+      <c r="R25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="18"/>
+      <c r="V25" s="18"/>
+      <c r="W25" s="18"/>
+      <c r="X25" s="18"/>
+      <c r="Y25" s="18"/>
+      <c r="Z25" s="18"/>
+      <c r="AA25" s="18"/>
+      <c r="AB25" s="18"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B26" s="15"/>
@@ -3982,37 +5994,37 @@
         <v>25</v>
       </c>
       <c r="P26" s="15"/>
-      <c r="R26" s="18" t="s">
+      <c r="R26" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="S26" s="19">
+      <c r="S26" s="18">
         <v>2</v>
       </c>
-      <c r="T26" s="19">
+      <c r="T26" s="18">
         <v>3</v>
       </c>
-      <c r="U26" s="19">
+      <c r="U26" s="18">
         <v>4</v>
       </c>
-      <c r="V26" s="19">
+      <c r="V26" s="18">
         <v>5</v>
       </c>
-      <c r="W26" s="19">
+      <c r="W26" s="18">
         <v>7</v>
       </c>
-      <c r="X26" s="19">
+      <c r="X26" s="18">
         <v>10</v>
       </c>
-      <c r="Y26" s="19">
+      <c r="Y26" s="18">
         <v>13</v>
       </c>
-      <c r="Z26" s="19">
+      <c r="Z26" s="18">
         <v>15</v>
       </c>
-      <c r="AA26" s="19">
+      <c r="AA26" s="18">
         <v>20</v>
       </c>
-      <c r="AB26" s="19">
+      <c r="AB26" s="18">
         <v>25</v>
       </c>
     </row>
@@ -4043,37 +6055,37 @@
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
-      <c r="R27" s="18" t="s">
+      <c r="R27" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="S27" s="20">
+      <c r="S27" s="19">
         <v>0.72159921989273501</v>
       </c>
-      <c r="T27" s="20">
+      <c r="T27" s="19">
         <v>0.76986835689907296</v>
       </c>
-      <c r="U27" s="20">
+      <c r="U27" s="19">
         <v>0.78595806923451905</v>
       </c>
-      <c r="V27" s="20">
+      <c r="V27" s="19">
         <v>0.80156021452949699</v>
       </c>
-      <c r="W27" s="20">
+      <c r="W27" s="19">
         <v>0.82593856655290099</v>
       </c>
-      <c r="X27" s="20">
+      <c r="X27" s="19">
         <v>0.83130180399804898</v>
       </c>
-      <c r="Y27" s="20">
+      <c r="Y27" s="19">
         <v>0.83666504144319798</v>
       </c>
-      <c r="Z27" s="20">
+      <c r="Z27" s="19">
         <v>0.83715260848366602</v>
       </c>
-      <c r="AA27" s="20">
+      <c r="AA27" s="19">
         <v>0.84056557776694196</v>
       </c>
-      <c r="AB27" s="20">
+      <c r="AB27" s="19">
         <v>0.84300341296928305</v>
       </c>
     </row>
@@ -4105,17 +6117,17 @@
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
-      <c r="R28" s="17"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="21"/>
-      <c r="U28" s="21"/>
-      <c r="V28" s="21"/>
-      <c r="W28" s="21"/>
-      <c r="X28" s="21"/>
-      <c r="Y28" s="21"/>
-      <c r="Z28" s="21"/>
-      <c r="AA28" s="21"/>
-      <c r="AB28" s="21"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="20"/>
+      <c r="U28" s="20"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="20"/>
+      <c r="X28" s="20"/>
+      <c r="Y28" s="20"/>
+      <c r="Z28" s="20"/>
+      <c r="AA28" s="20"/>
+      <c r="AB28" s="20"/>
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.25">
       <c r="E29" s="14" t="s">
@@ -4153,7 +6165,7 @@
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="E31" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="P31" s="15"/>
       <c r="R31" s="14"/>
@@ -4234,37 +6246,37 @@
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
-      <c r="R33" t="s">
-        <v>21</v>
-      </c>
-      <c r="S33" s="20">
+      <c r="R33" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="S33" s="22">
         <v>0.66192548561723796</v>
       </c>
-      <c r="T33" s="20">
+      <c r="T33" s="22">
         <v>0.72614372147330397</v>
       </c>
-      <c r="U33" s="20">
+      <c r="U33" s="22">
         <v>0.73813820188939605</v>
       </c>
-      <c r="V33" s="20">
+      <c r="V33" s="22">
         <v>0.75873049570109297</v>
       </c>
-      <c r="W33" s="20">
+      <c r="W33" s="22">
         <v>0.77560768495913401</v>
       </c>
-      <c r="X33" s="20">
+      <c r="X33" s="22">
         <v>0.779535081201571</v>
       </c>
-      <c r="Y33" s="20">
+      <c r="Y33" s="22">
         <v>0.78707143615327402</v>
       </c>
-      <c r="Z33" s="20">
+      <c r="Z33" s="22">
         <v>0.78983122810741901</v>
       </c>
-      <c r="AA33" s="20">
+      <c r="AA33" s="22">
         <v>0.79068039486254105</v>
       </c>
-      <c r="AB33" s="20">
+      <c r="AB33" s="22">
         <v>0.79407706188302696</v>
       </c>
     </row>
@@ -4295,37 +6307,37 @@
       <c r="N34" s="15"/>
       <c r="O34" s="15"/>
       <c r="P34" s="15"/>
-      <c r="R34" t="s">
-        <v>22</v>
-      </c>
-      <c r="S34" s="20">
+      <c r="R34" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="S34" s="22">
         <v>0.67141373683429695</v>
       </c>
-      <c r="T34" s="20">
+      <c r="T34" s="22">
         <v>0.72971369233051397</v>
       </c>
-      <c r="U34" s="20">
+      <c r="U34" s="22">
         <v>0.742471443406022</v>
       </c>
-      <c r="V34" s="20">
+      <c r="V34" s="22">
         <v>0.75789942145082301</v>
       </c>
-      <c r="W34" s="20">
+      <c r="W34" s="22">
         <v>0.77822281560599305</v>
       </c>
-      <c r="X34" s="20">
+      <c r="X34" s="22">
         <v>0.78742026405577803</v>
       </c>
-      <c r="Y34" s="20">
+      <c r="Y34" s="22">
         <v>0.79261237205162405</v>
       </c>
-      <c r="Z34" s="20">
+      <c r="Z34" s="22">
         <v>0.793502447708055</v>
       </c>
-      <c r="AA34" s="20">
+      <c r="AA34" s="22">
         <v>0.79735944221925503</v>
       </c>
-      <c r="AB34" s="20">
+      <c r="AB34" s="22">
         <v>0.79810117193294705</v>
       </c>
     </row>
@@ -4357,109 +6369,109 @@
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
       <c r="P35" s="15"/>
-      <c r="R35" t="s">
-        <v>23</v>
-      </c>
-      <c r="S35" s="20">
+      <c r="R35" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="S35" s="22">
         <v>0.67618813100221598</v>
       </c>
-      <c r="T35" s="20">
+      <c r="T35" s="22">
         <v>0.73947303619797999</v>
       </c>
-      <c r="U35" s="20">
+      <c r="U35" s="22">
         <v>0.75523270130509701</v>
       </c>
-      <c r="V35" s="20">
+      <c r="V35" s="22">
         <v>0.776409751292785</v>
       </c>
-      <c r="W35" s="20">
+      <c r="W35" s="22">
         <v>0.79857178034966703</v>
       </c>
-      <c r="X35" s="20">
+      <c r="X35" s="22">
         <v>0.80768283673971897</v>
       </c>
-      <c r="Y35" s="20">
+      <c r="Y35" s="22">
         <v>0.81113026348190098</v>
       </c>
-      <c r="Z35" s="20">
+      <c r="Z35" s="22">
         <v>0.81383895592218602</v>
       </c>
-      <c r="AA35" s="20">
+      <c r="AA35" s="22">
         <v>0.81383895592218602</v>
       </c>
-      <c r="AB35" s="20">
+      <c r="AB35" s="22">
         <v>0.81482393499138095</v>
       </c>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="R36" t="s">
-        <v>24</v>
-      </c>
-      <c r="S36" s="20">
+      <c r="R36" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="S36" s="22">
         <v>0.70562293274531396</v>
       </c>
-      <c r="T36" s="20">
+      <c r="T36" s="22">
         <v>0.76111723631018002</v>
       </c>
-      <c r="U36" s="20">
+      <c r="U36" s="22">
         <v>0.77471517824329295</v>
       </c>
-      <c r="V36" s="20">
+      <c r="V36" s="22">
         <v>0.79309077545020201</v>
       </c>
-      <c r="W36" s="20">
+      <c r="W36" s="22">
         <v>0.816244027930907</v>
       </c>
-      <c r="X36" s="20">
+      <c r="X36" s="22">
         <v>0.82102168320470403</v>
       </c>
-      <c r="Y36" s="20">
+      <c r="Y36" s="22">
         <v>0.82726938625505297</v>
       </c>
-      <c r="Z36" s="20">
+      <c r="Z36" s="22">
         <v>0.82800441014332904</v>
       </c>
-      <c r="AA36" s="20">
+      <c r="AA36" s="22">
         <v>0.83167952958471103</v>
       </c>
-      <c r="AB36" s="20">
+      <c r="AB36" s="22">
         <v>0.83094450569643497</v>
       </c>
     </row>
     <row r="37" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B37" s="15"/>
       <c r="P37" s="15"/>
-      <c r="R37" t="s">
-        <v>25</v>
-      </c>
-      <c r="S37" s="20">
+      <c r="R37" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="S37" s="22">
         <v>0.72159921989273501</v>
       </c>
-      <c r="T37" s="20">
+      <c r="T37" s="22">
         <v>0.76986835689907296</v>
       </c>
-      <c r="U37" s="20">
+      <c r="U37" s="22">
         <v>0.78595806923451905</v>
       </c>
-      <c r="V37" s="20">
+      <c r="V37" s="22">
         <v>0.80156021452949699</v>
       </c>
-      <c r="W37" s="20">
+      <c r="W37" s="22">
         <v>0.82593856655290099</v>
       </c>
-      <c r="X37" s="20">
+      <c r="X37" s="22">
         <v>0.83130180399804898</v>
       </c>
-      <c r="Y37" s="20">
+      <c r="Y37" s="22">
         <v>0.83666504144319798</v>
       </c>
-      <c r="Z37" s="20">
+      <c r="Z37" s="22">
         <v>0.83715260848366602</v>
       </c>
-      <c r="AA37" s="20">
+      <c r="AA37" s="22">
         <v>0.84056557776694196</v>
       </c>
-      <c r="AB37" s="20">
+      <c r="AB37" s="22">
         <v>0.84300341296928305</v>
       </c>
     </row>
@@ -4491,44 +6503,44 @@
       <c r="B50" s="15"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J51" t="s">
-        <v>21</v>
-      </c>
-      <c r="K51" s="15">
+      <c r="J51" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K51" s="22">
         <v>0.77949999999999997</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="15"/>
-      <c r="J52" t="s">
-        <v>22</v>
-      </c>
-      <c r="K52" s="15">
+      <c r="J52" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="K52" s="22">
         <v>0.78739999999999999</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J53" t="s">
-        <v>23</v>
-      </c>
-      <c r="K53" s="15">
+      <c r="J53" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K53" s="22">
         <v>0.80769999999999997</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="15"/>
-      <c r="J54" t="s">
-        <v>24</v>
-      </c>
-      <c r="K54" s="15">
+      <c r="J54" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K54" s="22">
         <v>0.82099999999999995</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J55" t="s">
-        <v>25</v>
-      </c>
-      <c r="K55" s="15">
+      <c r="J55" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="K55" s="22">
         <v>0.83130000000000004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Podzbiory cech - wykresy i tabela
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad1/wyniki.xlsx
+++ b/Sprawozdanie_zad1/wyniki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1581484C-444F-4C6F-89CD-7FBB574210E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7CAD82-39F6-4EE5-9087-4A2A466D39D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t>usa</t>
   </si>
@@ -117,6 +117,36 @@
   </si>
   <si>
     <t>k = 7</t>
+  </si>
+  <si>
+    <t>60 / 40</t>
+  </si>
+  <si>
+    <t>wszystkie</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>1, 3, 4, 7, 8</t>
+  </si>
+  <si>
+    <t>2, 5, 6, 9, 10</t>
+  </si>
+  <si>
+    <t>2, 4, 6, 8, 10</t>
+  </si>
+  <si>
+    <t>1, 3, 5, 7, 9</t>
   </si>
 </sst>
 </file>
@@ -2361,6 +2391,412 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="107"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="7"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz1!$O$95</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz1!$P$94:$T$94</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>wszystkie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1, 3, 4, 7, 8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2, 5, 6, 9, 10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2, 4, 6, 8, 10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1, 3, 5, 7, 9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz1!$P$95:$T$95</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.77718439400682404</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78653018839934696</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.77822281560599305</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.77288236166740798</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.77970627503337697</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8EBD-4F32-BC00-07066D1F340B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2069571232"/>
+        <c:axId val="2056057024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2069571232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+                  <a:t>Użyte cechy do klasyfikacji</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2056057024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2056057024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:t>Skuteczność (Accuracy)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2069571232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2518,6 +2954,12 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="25">
+  <a:schemeClr val="accent5"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3994,6 +4436,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4642,6 +5587,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Wykres 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9546B82-CDE8-4AD8-8138-D7990EB6FCAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4908,17 +5889,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI61"/>
+  <dimension ref="A1:AI95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+    <sheetView tabSelected="1" topLeftCell="H80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R94" sqref="R94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" customWidth="1"/>
     <col min="32" max="32" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6553,6 +7539,91 @@
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" s="15"/>
     </row>
+    <row r="87" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="M87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="M88" t="s">
+        <v>27</v>
+      </c>
+      <c r="O88" t="s">
+        <v>29</v>
+      </c>
+      <c r="P88" s="15">
+        <v>0.77718439400682404</v>
+      </c>
+    </row>
+    <row r="89" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="M89" t="s">
+        <v>11</v>
+      </c>
+      <c r="O89" t="s">
+        <v>30</v>
+      </c>
+      <c r="P89" s="15">
+        <v>0.78653018839934696</v>
+      </c>
+    </row>
+    <row r="90" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="O90" t="s">
+        <v>31</v>
+      </c>
+      <c r="P90" s="15">
+        <v>0.77822281560599305</v>
+      </c>
+    </row>
+    <row r="91" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="O91" t="s">
+        <v>32</v>
+      </c>
+      <c r="P91" s="15">
+        <v>0.77288236166740798</v>
+      </c>
+    </row>
+    <row r="92" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="O92" t="s">
+        <v>33</v>
+      </c>
+      <c r="P92" s="15">
+        <v>0.77970627503337697</v>
+      </c>
+    </row>
+    <row r="94" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="P94" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>34</v>
+      </c>
+      <c r="R94" t="s">
+        <v>35</v>
+      </c>
+      <c r="S94" t="s">
+        <v>36</v>
+      </c>
+      <c r="T94" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95" spans="13:20" x14ac:dyDescent="0.25">
+      <c r="P95" s="15">
+        <v>0.77718439400682404</v>
+      </c>
+      <c r="Q95" s="15">
+        <v>0.78653018839934696</v>
+      </c>
+      <c r="R95" s="15">
+        <v>0.77822281560599305</v>
+      </c>
+      <c r="S95" s="15">
+        <v>0.77288236166740798</v>
+      </c>
+      <c r="T95" s="15">
+        <v>0.77970627503337697</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added implementation for nGrams and Generalized Ngrams
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad1/wyniki.xlsx
+++ b/Sprawozdanie_zad1/wyniki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7CAD82-39F6-4EE5-9087-4A2A466D39D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8F557D-069C-47E5-A037-FC6C630AC469}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5385" yWindow="1395" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
   <si>
     <t>usa</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>1, 3, 5, 7, 9</t>
+  </si>
+  <si>
+    <t>z an</t>
+  </si>
+  <si>
+    <t>z ng</t>
   </si>
 </sst>
 </file>
@@ -5891,8 +5897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R94" sqref="R94"/>
+    <sheetView tabSelected="1" topLeftCell="P8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7106,8 +7112,12 @@
       <c r="R28" s="16"/>
       <c r="S28" s="20"/>
       <c r="T28" s="20"/>
-      <c r="U28" s="20"/>
-      <c r="V28" s="20"/>
+      <c r="U28" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="V28" s="20">
+        <v>0.80643588493417795</v>
+      </c>
       <c r="W28" s="20"/>
       <c r="X28" s="20"/>
       <c r="Y28" s="20"/>
@@ -7142,6 +7152,12 @@
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
+      <c r="U29" t="s">
+        <v>39</v>
+      </c>
+      <c r="V29" s="15">
+        <v>0.80643588493417795</v>
+      </c>
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B30" s="15"/>

</xml_diff>

<commit_message>
keywords - new method, info when launching programme
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad1/wyniki.xlsx
+++ b/Sprawozdanie_zad1/wyniki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8F557D-069C-47E5-A037-FC6C630AC469}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6811993-6B7A-48C1-AE80-6786B1929BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="1395" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
   <si>
     <t>usa</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>z ng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k </t>
+  </si>
+  <si>
+    <t>ngram</t>
   </si>
 </sst>
 </file>
@@ -5895,10 +5901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI95"/>
+  <dimension ref="A1:AI105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" topLeftCell="K4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB28" sqref="AB28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7555,12 +7561,12 @@
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" s="15"/>
     </row>
-    <row r="87" spans="13:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="12:20" x14ac:dyDescent="0.25">
       <c r="M87" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="13:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="12:20" x14ac:dyDescent="0.25">
       <c r="M88" t="s">
         <v>27</v>
       </c>
@@ -7571,7 +7577,7 @@
         <v>0.77718439400682404</v>
       </c>
     </row>
-    <row r="89" spans="13:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="12:20" x14ac:dyDescent="0.25">
       <c r="M89" t="s">
         <v>11</v>
       </c>
@@ -7582,7 +7588,7 @@
         <v>0.78653018839934696</v>
       </c>
     </row>
-    <row r="90" spans="13:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="12:20" x14ac:dyDescent="0.25">
       <c r="O90" t="s">
         <v>31</v>
       </c>
@@ -7590,7 +7596,7 @@
         <v>0.77822281560599305</v>
       </c>
     </row>
-    <row r="91" spans="13:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="12:20" x14ac:dyDescent="0.25">
       <c r="O91" t="s">
         <v>32</v>
       </c>
@@ -7598,7 +7604,8 @@
         <v>0.77288236166740798</v>
       </c>
     </row>
-    <row r="92" spans="13:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="12:20" x14ac:dyDescent="0.25">
+      <c r="L92" s="15"/>
       <c r="O92" t="s">
         <v>33</v>
       </c>
@@ -7606,39 +7613,155 @@
         <v>0.77970627503337697</v>
       </c>
     </row>
-    <row r="94" spans="13:20" x14ac:dyDescent="0.25">
-      <c r="P94" t="s">
+    <row r="94" spans="12:20" x14ac:dyDescent="0.25">
+      <c r="O94" s="21"/>
+      <c r="P94" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="Q94" t="s">
+      <c r="Q94" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="R94" t="s">
+      <c r="R94" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="S94" t="s">
+      <c r="S94" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="T94" t="s">
+      <c r="T94" s="21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="13:20" x14ac:dyDescent="0.25">
-      <c r="P95" s="15">
+    <row r="95" spans="12:20" x14ac:dyDescent="0.25">
+      <c r="O95" s="21"/>
+      <c r="P95" s="22">
         <v>0.77718439400682404</v>
       </c>
-      <c r="Q95" s="15">
+      <c r="Q95" s="22">
         <v>0.78653018839934696</v>
       </c>
-      <c r="R95" s="15">
+      <c r="R95" s="22">
         <v>0.77822281560599305</v>
       </c>
-      <c r="S95" s="15">
+      <c r="S95" s="22">
         <v>0.77288236166740798</v>
       </c>
-      <c r="T95" s="15">
+      <c r="T95" s="22">
         <v>0.77970627503337697</v>
       </c>
+    </row>
+    <row r="98" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>40</v>
+      </c>
+      <c r="E98">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>2</v>
+      </c>
+      <c r="F101">
+        <v>3</v>
+      </c>
+      <c r="G101">
+        <v>4</v>
+      </c>
+      <c r="H101">
+        <v>5</v>
+      </c>
+      <c r="I101">
+        <v>6</v>
+      </c>
+      <c r="J101">
+        <v>7</v>
+      </c>
+      <c r="K101">
+        <v>8</v>
+      </c>
+      <c r="L101">
+        <v>9</v>
+      </c>
+      <c r="M101">
+        <v>10</v>
+      </c>
+      <c r="N101">
+        <v>11</v>
+      </c>
+      <c r="O101" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="102" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D102" s="15">
+        <v>0.84349098000975098</v>
+      </c>
+      <c r="E102" s="15">
+        <v>0.84349098000975098</v>
+      </c>
+      <c r="F102" s="15">
+        <v>0.84056557776694196</v>
+      </c>
+      <c r="G102" s="15">
+        <v>0.84154071184787904</v>
+      </c>
+      <c r="H102" s="15">
+        <v>0.84397854705021902</v>
+      </c>
+      <c r="I102" s="15">
+        <v>0.83130180399804898</v>
+      </c>
+      <c r="J102" s="15">
+        <v>0.81082398829839097</v>
+      </c>
+      <c r="K102" s="15">
+        <v>0.81131155533885901</v>
+      </c>
+      <c r="L102" s="15">
+        <v>0.83471477328132604</v>
+      </c>
+      <c r="M102" s="15">
+        <v>0.83325207215992203</v>
+      </c>
+      <c r="N102" s="15">
+        <v>0.84495368113115499</v>
+      </c>
+      <c r="O102" s="15">
+        <v>0.80643588493417795</v>
+      </c>
+    </row>
+    <row r="103" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="I103" s="15"/>
+    </row>
+    <row r="104" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D104" s="15">
+        <v>0.84251584592881501</v>
+      </c>
+      <c r="N104" s="15">
+        <v>0.84495368113115499</v>
+      </c>
+      <c r="O104" s="15">
+        <v>0.81423695758166703</v>
+      </c>
+    </row>
+    <row r="105" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="I105" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ArticleGenerator->FileReader, sprawozdanie - wprowadzenie
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad1/wyniki.xlsx
+++ b/Sprawozdanie_zad1/wyniki.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6811993-6B7A-48C1-AE80-6786B1929BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C15A68D-7144-4A4C-B9D6-FD3D87E2B1B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
   <si>
     <t>usa</t>
   </si>
@@ -159,6 +160,66 @@
   </si>
   <si>
     <t>ngram</t>
+  </si>
+  <si>
+    <t>Settings: k=2 , training=30%, test=70%, metric=EuclideanMetric</t>
+  </si>
+  <si>
+    <t>Accuracy: 66,4154548349432%</t>
+  </si>
+  <si>
+    <t>Settings: k=3 , training=30%, test=70%, metric=EuclideanMetric</t>
+  </si>
+  <si>
+    <t>Accuracy: 73,32554930474473%</t>
+  </si>
+  <si>
+    <t>Settings: k=4 , training=30%, test=70%, metric=EuclideanMetric</t>
+  </si>
+  <si>
+    <t>Accuracy: 74,14287230654921%</t>
+  </si>
+  <si>
+    <t>Settings: k=5 , training=30%, test=70%, metric=EuclideanMetric</t>
+  </si>
+  <si>
+    <t>Accuracy: 76,22333085659696%</t>
+  </si>
+  <si>
+    <t>Settings: k=7 , training=30%, test=70%, metric=EuclideanMetric</t>
+  </si>
+  <si>
+    <t>Accuracy: 77,6775289247426%</t>
+  </si>
+  <si>
+    <t>Settings: k=10 , training=30%, test=70%, metric=EuclideanMetric</t>
+  </si>
+  <si>
+    <t>Accuracy: 77,99596645791317%</t>
+  </si>
+  <si>
+    <t>Settings: k=13 , training=30%, test=70%, metric=EuclideanMetric</t>
+  </si>
+  <si>
+    <t>Accuracy: 78,73898736864452%</t>
+  </si>
+  <si>
+    <t>Settings: k=15 , training=30%, test=70%, metric=EuclideanMetric</t>
+  </si>
+  <si>
+    <t>Accuracy: 79,01496656405902%</t>
+  </si>
+  <si>
+    <t>Settings: k=20 , training=30%, test=70%, metric=EuclideanMetric</t>
+  </si>
+  <si>
+    <t>Accuracy: 79,32278951279056%</t>
+  </si>
+  <si>
+    <t>Settings: k=25 , training=30%, test=70%, metric=EuclideanMetric</t>
+  </si>
+  <si>
+    <t>Accuracy: 79,41832077274175%</t>
   </si>
 </sst>
 </file>
@@ -5903,8 +5964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB28" sqref="AB28"/>
+    <sheetView topLeftCell="K4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6328,34 +6389,34 @@
         <v>9</v>
       </c>
       <c r="S11" s="19">
-        <v>0.66192548561723796</v>
+        <v>0.66415454834943199</v>
       </c>
       <c r="T11" s="19">
-        <v>0.72614372147330397</v>
+        <v>0.73325549304744697</v>
       </c>
       <c r="U11" s="19">
-        <v>0.73813820188939605</v>
+        <v>0.74142872306549201</v>
       </c>
       <c r="V11" s="19">
-        <v>0.75873049570109297</v>
+        <v>0.76223330856596905</v>
       </c>
       <c r="W11" s="19">
-        <v>0.77560768495913401</v>
+        <v>0.776775289247426</v>
       </c>
       <c r="X11" s="19">
-        <v>0.779535081201571</v>
+        <v>0.77995966457913102</v>
       </c>
       <c r="Y11" s="19">
-        <v>0.78707143615327402</v>
+        <v>0.78738987368644497</v>
       </c>
       <c r="Z11" s="19">
-        <v>0.78983122810741901</v>
+        <v>0.79014966564058997</v>
       </c>
       <c r="AA11" s="19">
-        <v>0.79068039486254105</v>
+        <v>0.79322789512790504</v>
       </c>
       <c r="AB11" s="19">
-        <v>0.79407706188302696</v>
+        <v>0.79418320772741702</v>
       </c>
       <c r="AF11" s="21"/>
       <c r="AG11" s="21" t="s">
@@ -7767,4 +7828,119 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB85EF92-5DCD-4B24-BBA6-E22CA62C4677}">
+  <dimension ref="F13:F32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="13" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added accuracy precision recall implementation, report without discussion and conlusions
</commit_message>
<xml_diff>
--- a/Sprawozdanie_zad1/wyniki.xlsx
+++ b/Sprawozdanie_zad1/wyniki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xd\inf\6 semestr\Komputerowe systemy rozpoznawania\KSR git\Sprawozdanie_zad1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C15A68D-7144-4A4C-B9D6-FD3D87E2B1B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49168C2D-C144-473F-B93B-FCDB85654E36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9540" yWindow="1230" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="65">
   <si>
     <t>usa</t>
   </si>
@@ -162,71 +162,80 @@
     <t>ngram</t>
   </si>
   <si>
-    <t>Settings: k=2 , training=30%, test=70%, metric=EuclideanMetric</t>
+    <t>predicted</t>
   </si>
   <si>
-    <t>Accuracy: 66,4154548349432%</t>
+    <t>recall</t>
   </si>
   <si>
-    <t>Settings: k=3 , training=30%, test=70%, metric=EuclideanMetric</t>
+    <t>precision</t>
   </si>
   <si>
-    <t>Accuracy: 73,32554930474473%</t>
+    <t>real</t>
   </si>
   <si>
-    <t>Settings: k=4 , training=30%, test=70%, metric=EuclideanMetric</t>
+    <t xml:space="preserve">2 &amp; 67,705 \\ </t>
   </si>
   <si>
-    <t>Accuracy: 74,14287230654921%</t>
+    <t>3 &amp; 73,921 \\</t>
   </si>
   <si>
-    <t>Settings: k=5 , training=30%, test=70%, metric=EuclideanMetric</t>
+    <t>4 &amp; 74,900 \\</t>
   </si>
   <si>
-    <t>Accuracy: 76,22333085659696%</t>
+    <t>5 &amp; 76,799 \\</t>
   </si>
   <si>
-    <t>Settings: k=7 , training=30%, test=70%, metric=EuclideanMetric</t>
+    <t>7 &amp; 78,312 \\</t>
   </si>
   <si>
-    <t>Accuracy: 77,6775289247426%</t>
+    <t>10 &amp; 79,024 \\</t>
   </si>
   <si>
-    <t>Settings: k=10 , training=30%, test=70%, metric=EuclideanMetric</t>
+    <t>13 &amp; 79,365 \\</t>
   </si>
   <si>
-    <t>Accuracy: 77,99596645791317%</t>
+    <t>15 &amp; 79,410 \\</t>
   </si>
   <si>
-    <t>Settings: k=13 , training=30%, test=70%, metric=EuclideanMetric</t>
+    <t>20 &amp; 79,632 \\</t>
   </si>
   <si>
-    <t>Accuracy: 78,73898736864452%</t>
+    <t>25 &amp; 79,795 \\</t>
   </si>
   <si>
-    <t>Settings: k=15 , training=30%, test=70%, metric=EuclideanMetric</t>
+    <t>k = 10</t>
   </si>
   <si>
-    <t>Accuracy: 79,01496656405902%</t>
+    <t>k = 13</t>
   </si>
   <si>
-    <t>Settings: k=20 , training=30%, test=70%, metric=EuclideanMetric</t>
+    <t>Manhattan</t>
   </si>
   <si>
-    <t>Accuracy: 79,32278951279056%</t>
+    <t>Czebyszewa</t>
   </si>
   <si>
-    <t>Settings: k=25 , training=30%, test=70%, metric=EuclideanMetric</t>
+    <t>Euklidesowa</t>
   </si>
   <si>
-    <t>Accuracy: 79,41832077274175%</t>
+    <t>1, 2, 3, 4 ,5, 11</t>
+  </si>
+  <si>
+    <t>6, 7, 8, 9, 10</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 8, 9, 10</t>
+  </si>
+  <si>
+    <t>4, 5, 6, 7, 11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,8 +243,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +266,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE3DE00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -372,6 +405,34 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -2870,6 +2931,1506 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Arkusz2!$C$4:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz2!$H$4:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>67.704999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73.921000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76.799000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78.311999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>79.024000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.364999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>79.41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>79.632000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79.795000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B8F9-4379-B76B-192E58888743}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1662401952"/>
+        <c:axId val="1526421040"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1662401952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400" baseline="0"/>
+                  <a:t>k</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1526421040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1526421040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400"/>
+                  <a:t>Accuracy [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1662401952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz2!$C$38:$C$42</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30 / 70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50 / 50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70 / 30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80 / 20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85 / 15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz2!$D$38:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>78.325000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>78.978999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.409000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.911000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.667000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-33A2-4A4E-A717-0F0492A71656}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1658643312"/>
+        <c:axId val="1528595904"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1658643312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400"/>
+                  <a:t>Podział na dane treningowe/testowe</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1528595904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1528595904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400"/>
+                  <a:t>Accuracy [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1658643312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz2!$C$46:$C$48</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Manhattan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Czebyszewa</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Euklidesowa</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz2!$D$46:$D$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>81.384</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81.334999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.409000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D42B-48AF-A1C5-CE533CA3D751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1662415152"/>
+        <c:axId val="1878503024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1662415152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400"/>
+                  <a:t>Metryka</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1878503024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1878503024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400"/>
+                  <a:t>Accuracy [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1662415152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Arkusz2!$X$19:$X$23</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>wszystkie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1, 2, 3, 4 ,5, 11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6, 7, 8, 9, 10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1, 2, 3, 8, 9, 10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4, 5, 6, 7, 11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz2!$Y$19:$Y$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>79.572999999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79.81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.558000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79.662000000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79.78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5C7A-4DC5-965F-5A4D3664AAED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1881842192"/>
+        <c:axId val="1878503440"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1881842192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400"/>
+                  <a:t>Podzbiór</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400" baseline="0"/>
+                  <a:t> cech</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1878503440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1878503440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="1400"/>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t> [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1881842192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3033,6 +4594,160 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5012,6 +6727,2018 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5699,6 +9426,155 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FB1683D-2E2C-42E5-99E8-4D6F6B0344D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>657224</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Wykres 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43C86853-96FB-49C8-BA93-034836DACF6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D78EBFEF-742F-4B51-BF82-3D969388125E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Wykres 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD1215C6-9F4D-4496-A53B-D24F0AB3A611}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5964,13 +9840,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI105"/>
   <sheetViews>
-    <sheetView topLeftCell="K4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" customWidth="1"/>
     <col min="16" max="16" width="10.85546875" customWidth="1"/>
@@ -5985,18 +9862,23 @@
       <c r="A1" s="5">
         <v>322</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>3</v>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6">
+        <v>10685</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>10685</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="10"/>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="33">
+        <v>812</v>
+      </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -6068,10 +9950,12 @@
       <c r="A3" s="7">
         <v>251</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="33">
+        <v>251</v>
+      </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -6159,24 +10043,33 @@
       <c r="A4" s="7">
         <v>905</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>5</v>
+      <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>466</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>812</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>1</v>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>466</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
+      <c r="B6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>905</v>
       </c>
       <c r="R6" t="s">
         <v>17</v>
@@ -7832,115 +11725,681 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB85EF92-5DCD-4B24-BBA6-E22CA62C4677}">
-  <dimension ref="F13:F32"/>
+  <dimension ref="B3:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="L9" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" customWidth="1"/>
+    <col min="24" max="24" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="13" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
+    <row r="3" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C4" s="21">
+        <v>2</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="str">
+        <f>MID(D4,5,35)</f>
+        <v xml:space="preserve">67,705 \\ </v>
+      </c>
+      <c r="G4" s="34" t="str">
+        <f>LEFT(F4,7)</f>
+        <v xml:space="preserve">67,705 </v>
+      </c>
+      <c r="H4" s="21">
+        <f>VALUE(G4)</f>
+        <v>67.704999999999998</v>
+      </c>
+      <c r="M4" s="28"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="37"/>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C5" s="21">
+        <v>3</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="str">
+        <f>MID(D5,5,35)</f>
+        <v>73,921 \\</v>
+      </c>
+      <c r="G5" s="34" t="str">
+        <f>LEFT(F5,7)</f>
+        <v xml:space="preserve">73,921 </v>
+      </c>
+      <c r="H5" s="21">
+        <f>VALUE(G5)</f>
+        <v>73.921000000000006</v>
+      </c>
+      <c r="M5" s="29"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="8"/>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C6" s="21">
+        <v>4</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F13" si="0">MID(D6,5,35)</f>
+        <v>74,900 \\</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ref="G6:G13" si="1">LEFT(F6,7)</f>
+        <v xml:space="preserve">74,900 </v>
+      </c>
+      <c r="H6" s="21">
+        <f t="shared" ref="H6:H13" si="2">VALUE(G6)</f>
+        <v>74.900000000000006</v>
+      </c>
+      <c r="M6" s="29"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="T6" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="V6" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C7" s="21">
+        <v>5</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>76,799 \\</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">76,799 </v>
+      </c>
+      <c r="H7" s="21">
+        <f t="shared" si="2"/>
+        <v>76.799000000000007</v>
+      </c>
+      <c r="M7" s="38" t="s">
         <v>42</v>
       </c>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" s="26">
+        <v>1345</v>
+      </c>
+      <c r="Q7" s="25">
+        <v>3</v>
+      </c>
+      <c r="R7" s="25">
+        <v>9</v>
+      </c>
+      <c r="S7" s="10">
+        <v>123</v>
+      </c>
+      <c r="T7" s="10">
+        <v>1</v>
+      </c>
+      <c r="U7" s="8">
+        <v>122</v>
+      </c>
+      <c r="V7" s="32">
+        <f>P7/SUM(P7:U7)</f>
+        <v>0.83905177791640673</v>
+      </c>
     </row>
-    <row r="14" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C8" s="21">
+        <v>7</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>78,312 \\</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">78,312 </v>
+      </c>
+      <c r="H8" s="21">
+        <f t="shared" si="2"/>
+        <v>78.311999999999998</v>
+      </c>
+      <c r="M8" s="38"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="26">
+        <v>4</v>
+      </c>
+      <c r="R8" s="25">
+        <v>7</v>
+      </c>
+      <c r="S8" s="10">
+        <v>231</v>
+      </c>
+      <c r="T8" s="10">
+        <v>1</v>
+      </c>
+      <c r="U8" s="8">
+        <v>2</v>
+      </c>
+      <c r="V8" s="32">
+        <f t="shared" ref="V8:V12" si="3">P8/SUM(P8:U8)</f>
+        <v>1.2096774193548387E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C9" s="21">
+        <v>10</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 79,024 \\</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> 79,024</v>
+      </c>
+      <c r="H9" s="21">
+        <f t="shared" si="2"/>
+        <v>79.024000000000001</v>
+      </c>
+      <c r="M9" s="38"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="25">
+        <v>5</v>
+      </c>
+      <c r="R9" s="26">
+        <v>574</v>
+      </c>
+      <c r="S9" s="10">
+        <v>23</v>
+      </c>
+      <c r="T9" s="10">
+        <v>12</v>
+      </c>
+      <c r="U9" s="8">
+        <v>312</v>
+      </c>
+      <c r="V9" s="32">
+        <f t="shared" si="3"/>
+        <v>4.3010752688172043E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C10" s="21">
+        <v>13</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 79,365 \\</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> 79,365</v>
+      </c>
+      <c r="H10" s="21">
+        <f t="shared" si="2"/>
+        <v>79.364999999999995</v>
+      </c>
+      <c r="M10" s="38"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>6</v>
+      </c>
+      <c r="R10" s="10">
+        <v>57</v>
+      </c>
+      <c r="S10" s="26">
+        <v>3</v>
+      </c>
+      <c r="T10" s="10">
+        <v>4</v>
+      </c>
+      <c r="U10" s="8">
+        <v>5</v>
+      </c>
+      <c r="V10" s="32">
+        <f t="shared" si="3"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C11" s="21">
+        <v>15</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 79,410 \\</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> 79,410</v>
+      </c>
+      <c r="H11" s="21">
+        <f t="shared" si="2"/>
+        <v>79.41</v>
+      </c>
+      <c r="M11" s="38"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="10">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>7</v>
+      </c>
+      <c r="R11" s="10">
+        <v>457</v>
+      </c>
+      <c r="S11" s="10">
+        <v>4</v>
+      </c>
+      <c r="T11" s="26">
+        <v>3</v>
+      </c>
+      <c r="U11" s="8">
+        <v>4</v>
+      </c>
+      <c r="V11" s="32">
+        <f t="shared" si="3"/>
+        <v>1.2474012474012475E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="21">
+        <v>20</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 79,632 \\</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> 79,632</v>
+      </c>
+      <c r="H12" s="21">
+        <f t="shared" si="2"/>
+        <v>79.632000000000005</v>
+      </c>
+      <c r="M12" s="39"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>8</v>
+      </c>
+      <c r="R12" s="3">
+        <v>457</v>
+      </c>
+      <c r="S12" s="3">
+        <v>122</v>
+      </c>
+      <c r="T12" s="3">
+        <v>5</v>
+      </c>
+      <c r="U12" s="27">
+        <v>222</v>
+      </c>
+      <c r="V12" s="32">
+        <f t="shared" si="3"/>
+        <v>8.5261875761266752E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C13" s="21">
+        <v>25</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 79,795 \\</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> 79,795</v>
+      </c>
+      <c r="H13" s="21">
+        <f t="shared" si="2"/>
+        <v>79.795000000000002</v>
+      </c>
+      <c r="O13" s="30" t="s">
         <v>43</v>
       </c>
+      <c r="P13" s="32">
+        <f>P7/SUM(P7:P12)</f>
+        <v>0.98175182481751821</v>
+      </c>
+      <c r="Q13" s="32">
+        <f t="shared" ref="Q13:U13" si="4">Q7/SUM(Q7:Q12)</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="R13" s="32">
+        <f t="shared" si="4"/>
+        <v>5.7655349135169766E-3</v>
+      </c>
+      <c r="S13" s="32">
+        <f t="shared" si="4"/>
+        <v>0.24308300395256918</v>
+      </c>
+      <c r="T13" s="32">
+        <f t="shared" si="4"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="U13" s="32">
+        <f t="shared" si="4"/>
+        <v>0.18290854572713644</v>
+      </c>
     </row>
-    <row r="15" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
         <v>44</v>
       </c>
+      <c r="Q15" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="16" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F16" t="s">
-        <v>45</v>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="O16" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" s="15">
+        <f>V7</f>
+        <v>0.83905177791640673</v>
+      </c>
+      <c r="Q16" s="15">
+        <f>P13</f>
+        <v>0.98175182481751821</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" t="s">
-        <v>46</v>
+    <row r="17" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="O17" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="P17" s="15">
+        <f t="shared" ref="P17:P21" si="5">V8</f>
+        <v>1.2096774193548387E-2</v>
+      </c>
+      <c r="Q17" s="15">
+        <f>Q13</f>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
-        <v>47</v>
+    <row r="18" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="O18" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="P18" s="15">
+        <f t="shared" si="5"/>
+        <v>4.3010752688172043E-3</v>
+      </c>
+      <c r="Q18" s="15">
+        <f>R13</f>
+        <v>5.7655349135169766E-3</v>
       </c>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" t="s">
-        <v>48</v>
+    <row r="19" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="O19" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P19" s="15">
+        <f t="shared" si="5"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q19" s="15">
+        <f>S13</f>
+        <v>0.24308300395256918</v>
+      </c>
+      <c r="X19" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y19">
+        <v>79.572999999999993</v>
       </c>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
-        <v>49</v>
+    <row r="20" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="O20" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="P20" s="15">
+        <f t="shared" si="5"/>
+        <v>1.2474012474012475E-2</v>
+      </c>
+      <c r="Q20" s="15">
+        <f>T13</f>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="X20" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y20">
+        <v>79.81</v>
       </c>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" t="s">
-        <v>50</v>
+    <row r="21" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="O21" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="P21" s="15">
+        <f t="shared" si="5"/>
+        <v>8.5261875761266752E-3</v>
+      </c>
+      <c r="Q21" s="15">
+        <f>U13</f>
+        <v>0.18290854572713644</v>
+      </c>
+      <c r="X21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y21">
+        <v>79.558000000000007</v>
       </c>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>51</v>
+    <row r="22" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="X22" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y22">
+        <v>79.662000000000006</v>
       </c>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
-        <v>52</v>
+    <row r="23" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="X23" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y23">
+        <v>79.78</v>
       </c>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
-        <v>53</v>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" t="s">
-        <v>54</v>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" t="s">
-        <v>55</v>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>78.325000000000003</v>
       </c>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27" t="s">
-        <v>56</v>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39">
+        <v>78.978999999999999</v>
       </c>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40">
+        <v>81.409000000000006</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41">
+        <v>82.911000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>83.667000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
         <v>58</v>
       </c>
+      <c r="D46">
+        <v>81.384</v>
+      </c>
     </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
         <v>59</v>
       </c>
+      <c r="D47">
+        <v>81.334999999999994</v>
+      </c>
     </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
-        <v>61</v>
+      <c r="D48">
+        <v>81.409000000000006</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="M7:M12"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>